<commit_message>
Se agrega al plan de testeo los modulos registrar producto
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21255" windowHeight="9975" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21255" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Wildo" sheetId="1" r:id="rId1"/>
     <sheet name="Raul" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="192">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -460,6 +460,138 @@
   </si>
   <si>
     <t>Sale de la interfaz y va a la pagina principal</t>
+  </si>
+  <si>
+    <t>Hacer click en boton cancelar</t>
+  </si>
+  <si>
+    <t>Debe redireccionar a la pagina principal</t>
+  </si>
+  <si>
+    <t>Hacer click en el boton limpiar</t>
+  </si>
+  <si>
+    <t>Debe limpiar todos los campos de la pagina</t>
+  </si>
+  <si>
+    <t>Buscar por rango de fechas y por numero de nota</t>
+  </si>
+  <si>
+    <t>Debe aparecer solo una nota de retiro porque los numeros no se repiten</t>
+  </si>
+  <si>
+    <t>Buscar por rango de fechas y estado</t>
+  </si>
+  <si>
+    <t>Debe aparecer todas las notas de retiro en ese rango y con ese estado</t>
+  </si>
+  <si>
+    <t>Producto --&gt; Registrar Producto</t>
+  </si>
+  <si>
+    <t>Ingresar el numero de la hoja de ruta (Debe aparecer en el autocomplete el numero )</t>
+  </si>
+  <si>
+    <t>Debe setear automaticamente los siguientes campos:</t>
+  </si>
+  <si>
+    <t>Cliente, cantidad producto, item, tipo producto, remitente</t>
+  </si>
+  <si>
+    <t>Seleccionar un destinatario(aparecen las opciones ingresando 3 letras en el autocomplete)</t>
+  </si>
+  <si>
+    <t>Debe aparecer todas las direcciones para ese destinatario</t>
+  </si>
+  <si>
+    <t>Seleccionar direccion</t>
+  </si>
+  <si>
+    <t>Debe aparecer automaticamente la ciudad y luego el focus debe estar sobre</t>
+  </si>
+  <si>
+    <t>el codigo de barras</t>
+  </si>
+  <si>
+    <t>Ingresar el codigo de barras con el lector</t>
+  </si>
+  <si>
+    <t>Debe guardar automaticamente el producto , el item incrementa en 1</t>
+  </si>
+  <si>
+    <t>registrar</t>
+  </si>
+  <si>
+    <t>Solo puede guardar el maximo "Cantidad productos"</t>
+  </si>
+  <si>
+    <t>Controlar que se guarde max la cantidad de productos a registrar</t>
+  </si>
+  <si>
+    <t>Ingresar otro numero de nota que tenga registrados algunos de sus productos</t>
+  </si>
+  <si>
+    <t>Debe aparecer una lista de todos los productos registrados anteriormente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, el item debe empezar con el numero siguiente a registrar </t>
+  </si>
+  <si>
+    <t>Registrar un nuevo destinatario y guardar el producto con este.</t>
+  </si>
+  <si>
+    <t>Registrar un producto con un destinatario existente, luego el proximo con un nuevo destinatario</t>
+  </si>
+  <si>
+    <t>y el tercer producto con otro nuevo destinatario</t>
+  </si>
+  <si>
+    <t>No debe haber problemas, los productos deben guardarse correctamente</t>
+  </si>
+  <si>
+    <t>Deben saltar las validaciones</t>
+  </si>
+  <si>
+    <t>Hacer click en guardar sin ningun campo cargado y mirar en consola</t>
+  </si>
+  <si>
+    <t>Hace clcik en cancelar</t>
+  </si>
+  <si>
+    <t>Debe volver a la pagina principal</t>
+  </si>
+  <si>
+    <t>No debe permitir el sistema, debe aparecer un mensaje: ""</t>
+  </si>
+  <si>
+    <t>Guardar el producto con un codigo de barra ya existente</t>
+  </si>
+  <si>
+    <t>Atencion!!El codigo ingresado ya fue registrado.</t>
+  </si>
+  <si>
+    <t>Intentar ingresar letras en campos numericos</t>
+  </si>
+  <si>
+    <t>No debe permitir porque solo se aceptan numeros</t>
+  </si>
+  <si>
+    <t>El campo codigo de barra solo acepta hasta 25 numeros</t>
+  </si>
+  <si>
+    <t>No debe permitir agregar mas de esta cantidad ni ingresar letras</t>
+  </si>
+  <si>
+    <t>Descripcion acepta hasta 100 caracteres</t>
+  </si>
+  <si>
+    <t>Eliminar un producto de la lista de productos registrados</t>
+  </si>
+  <si>
+    <t>El producto debe eliminarse de la lista y de la bd. El item debe disminuir en 1</t>
+  </si>
+  <si>
+    <t>Aplicar tus propias formas de testear</t>
   </si>
 </sst>
 </file>
@@ -803,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1262,12 +1394,261 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>6</v>
       </c>
       <c r="B65" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="C73" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
+        <v>162</v>
+      </c>
+      <c r="C75" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="C76" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>4</v>
+      </c>
+      <c r="B77" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>170</v>
+      </c>
+      <c r="C80" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="C81" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="B84" t="s">
+        <v>175</v>
+      </c>
+      <c r="C84" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>9</v>
+      </c>
+      <c r="B86" t="s">
+        <v>178</v>
+      </c>
+      <c r="C86" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>10</v>
+      </c>
+      <c r="B87" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>11</v>
+      </c>
+      <c r="B88" t="s">
+        <v>182</v>
+      </c>
+      <c r="C88" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="C89" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>12</v>
+      </c>
+      <c r="B90" t="s">
+        <v>184</v>
+      </c>
+      <c r="C90" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>13</v>
+      </c>
+      <c r="B91" t="s">
+        <v>186</v>
+      </c>
+      <c r="C91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>14</v>
+      </c>
+      <c r="B92" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>15</v>
+      </c>
+      <c r="B93" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>16</v>
+      </c>
+      <c r="B94" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1280,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualizacion del Plan de Testeo (Destinatarios y Usuarios)
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="21255" windowHeight="9975"/>
@@ -11,12 +11,12 @@
     <sheet name="Raul" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="231">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -592,13 +592,130 @@
   </si>
   <si>
     <t>Aplicar tus propias formas de testear</t>
+  </si>
+  <si>
+    <t>Destinatarios</t>
+  </si>
+  <si>
+    <t>Leois Linka</t>
+  </si>
+  <si>
+    <t>Ingresar un destinatario con con todos los campos obligatorios</t>
+  </si>
+  <si>
+    <t>y limpiar los campos del formulario</t>
+  </si>
+  <si>
+    <t>Registrar un cliente sin ingresar al menos una direccion.</t>
+  </si>
+  <si>
+    <t>al menos debe contener una direccion</t>
+  </si>
+  <si>
+    <t>Hacer click en agregar sin setear los campos correspondientes a la direccion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No debe agregar la direccion en la tabla de direcciones  a la derecha del </t>
+  </si>
+  <si>
+    <t>formulario</t>
+  </si>
+  <si>
+    <t>No debe permitir eliminar un destinatario que esta siendo usado</t>
+  </si>
+  <si>
+    <t>Eliminar un destinatario con referencias a otros modelos</t>
+  </si>
+  <si>
+    <t>Eliminar destinatarios sin referencias a otros modelos</t>
+  </si>
+  <si>
+    <t>Aparece un mensaje de confirmacion, preguntando si realmente desea</t>
+  </si>
+  <si>
+    <t>eliminar el destinatario</t>
+  </si>
+  <si>
+    <t>Nombre y Apellido: max cantidad de caracteres 50</t>
+  </si>
+  <si>
+    <t>Nro de Documento: max cantidad de caracteres 20</t>
+  </si>
+  <si>
+    <t>Lugar: max cantidad de caracteres 15</t>
+  </si>
+  <si>
+    <t>Ciudad: debe ser un autocomplete</t>
+  </si>
+  <si>
+    <t>Dirección:  texto</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Ingresar un usuario con con todos los campos obligatorios</t>
+  </si>
+  <si>
+    <t>Debe guardar el usuario, mostrarlo en la tabla inferior</t>
+  </si>
+  <si>
+    <t>Debe guardar el destinatario mostrarlo en la tabla inferior</t>
+  </si>
+  <si>
+    <t>Registrar un usuario, sin ingresar todos los campos obligariorios</t>
+  </si>
+  <si>
+    <t>No debe de guardarse el cliente, las validaciones aparecen en rojo</t>
+  </si>
+  <si>
+    <t>No se habilita el boton guardar</t>
+  </si>
+  <si>
+    <t>Registrar un usuario sin ningun rol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No debe guardar el destintario. Debe mostrar un mensaje informando que </t>
+  </si>
+  <si>
+    <t>No debe guardar el usuario. No se habilita el boton guardar</t>
+  </si>
+  <si>
+    <t>Eliminar un usuario con referencias a otros modelos</t>
+  </si>
+  <si>
+    <t>No debe permitir eliminar un usuario que esta siendo usado</t>
+  </si>
+  <si>
+    <t>Eliminar usuarios sin referencias a otros modelos</t>
+  </si>
+  <si>
+    <t>eliminar el usuario</t>
+  </si>
+  <si>
+    <t>Empleado: autocomplete</t>
+  </si>
+  <si>
+    <t>Usuario: max cantidad de caracteres 20</t>
+  </si>
+  <si>
+    <t>Email: max cantidad de caracteres 50</t>
+  </si>
+  <si>
+    <t>Contraseña: no tiene limite</t>
+  </si>
+  <si>
+    <t>Confirmar contraseña: no tiene limite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,10 +726,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -651,7 +772,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -935,13 +1056,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="81.85546875" customWidth="1"/>
@@ -1651,7 +1772,285 @@
         <v>191</v>
       </c>
     </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="B99" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="C101" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>2</v>
+      </c>
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="C104" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>3</v>
+      </c>
+      <c r="B106" t="s">
+        <v>196</v>
+      </c>
+      <c r="C106" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="C107" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110">
+        <v>4</v>
+      </c>
+      <c r="B110" t="s">
+        <v>198</v>
+      </c>
+      <c r="C110" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="C111" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113">
+        <v>5</v>
+      </c>
+      <c r="B113" t="s">
+        <v>202</v>
+      </c>
+      <c r="C113" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115">
+        <v>6</v>
+      </c>
+      <c r="B115" t="s">
+        <v>203</v>
+      </c>
+      <c r="C115" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="C116" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>26</v>
+      </c>
+      <c r="C118" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="C119" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="C120" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="C121" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="C122" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="C123" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="B126" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127">
+        <v>1</v>
+      </c>
+      <c r="B127" t="s">
+        <v>213</v>
+      </c>
+      <c r="C127" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="C128" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130">
+        <v>2</v>
+      </c>
+      <c r="B130" t="s">
+        <v>216</v>
+      </c>
+      <c r="C130" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="C131" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133">
+        <v>3</v>
+      </c>
+      <c r="B133" t="s">
+        <v>219</v>
+      </c>
+      <c r="C133" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140">
+        <v>4</v>
+      </c>
+      <c r="B140" t="s">
+        <v>222</v>
+      </c>
+      <c r="C140" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142">
+        <v>5</v>
+      </c>
+      <c r="B142" t="s">
+        <v>224</v>
+      </c>
+      <c r="C142" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="C143" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145">
+        <v>6</v>
+      </c>
+      <c r="B145" t="s">
+        <v>26</v>
+      </c>
+      <c r="C145" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="C146" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="C147" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="C148" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="C149" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1665,7 +2064,7 @@
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
@@ -2543,6 +2942,7 @@
       <c r="C168" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
@@ -2554,8 +2954,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion del plan de testeo
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="271">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -709,6 +709,126 @@
   </si>
   <si>
     <t>Confirmar contraseña: no tiene limite</t>
+  </si>
+  <si>
+    <t>Cada rol accede a modulos especificos a los que tiene permiso</t>
+  </si>
+  <si>
+    <t>un usuario, de ninguna forma debe obtener acceso un modulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> que no esta asignado a su rol o a sus roles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permisos de Secreataria: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, CargoManifest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :anage, CargoManifestDetail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, Country </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, Customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, CustomerType </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, PaymentMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, ProductState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, ProductType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, Province</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, Receiver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, ReceiverAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, RetireNote </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, RetireNoteState </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, RoutingSheet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, RoutingSheetDetail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, RoutingSheetState </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, ServiceType </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, TransportGuide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, TransportGuideDetail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, TransportGuideState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           can :manage, Area</t>
+  </si>
+  <si>
+    <t>Permisos de Entregador:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            can :manage, RoutingSheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            can :manage, RoutingSheetDetail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            can :manage, RoutingSheetState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permisos de Administrador: </t>
+  </si>
+  <si>
+    <t>El administrador puede acceder a todos los modulos del sistema</t>
+  </si>
+  <si>
+    <t>Que pueda acceder a cada uno de estos modulos y ningun otro.</t>
+  </si>
+  <si>
+    <t>Timeout</t>
+  </si>
+  <si>
+    <t>Cada 10 minutos debe hacer un timeout, debe pedir al usuario que se loguee</t>
+  </si>
+  <si>
+    <t>luego deve volver a la misma pagina donde se encontraba cuando</t>
+  </si>
+  <si>
+    <t>se expiro la session.</t>
+  </si>
+  <si>
+    <t>Roles y Permisos</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2018,7 +2138,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:4">
       <c r="A145">
         <v>6</v>
       </c>
@@ -2029,24 +2149,248 @@
         <v>226</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:4">
       <c r="C146" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:4">
       <c r="C147" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:4">
       <c r="C148" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:4">
       <c r="C149" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="B152" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D152" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153">
+        <v>1</v>
+      </c>
+      <c r="B153" t="s">
+        <v>231</v>
+      </c>
+      <c r="C153" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="C154" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156">
+        <v>2</v>
+      </c>
+      <c r="B156" t="s">
+        <v>263</v>
+      </c>
+      <c r="C156" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158">
+        <v>3</v>
+      </c>
+      <c r="B158" t="s">
+        <v>234</v>
+      </c>
+      <c r="C158" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="B159" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="B160" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2">
+      <c r="B163" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2">
+      <c r="B165" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2">
+      <c r="B174" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2">
+      <c r="B175" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2">
+      <c r="B176" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="B177" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="B178" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="B179" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="B180" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="B181" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="B182" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184">
+        <v>4</v>
+      </c>
+      <c r="B184" t="s">
+        <v>259</v>
+      </c>
+      <c r="C184" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="B185" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="B186" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="B187" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189">
+        <v>5</v>
+      </c>
+      <c r="B189" t="s">
+        <v>266</v>
+      </c>
+      <c r="C189" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="C190" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="C191" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega al plan de testeo el modulo de hoja de ruta
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="21255" windowHeight="9975"/>
@@ -11,12 +11,12 @@
     <sheet name="Raul" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="306">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -829,13 +829,118 @@
   </si>
   <si>
     <t>Roles y Permisos</t>
+  </si>
+  <si>
+    <t>1) Guardar una hoja de ruta sin detalles</t>
+  </si>
+  <si>
+    <t>El boton guardar no debe habilitarse, en caso de hackear el javascript</t>
+  </si>
+  <si>
+    <t>del boton guardar el servidor muestra un mensaje:</t>
+  </si>
+  <si>
+    <t>"Prohibido guardar sin agregar algun producto..", validado en el servidor</t>
+  </si>
+  <si>
+    <t>2)En el campo codigo: ingresar 10 codigos de barra de productos en estado="No Enviado"</t>
+  </si>
+  <si>
+    <t>Debe aparecer en la lista de los detalles los 10 productos en el orden</t>
+  </si>
+  <si>
+    <t>que se fueron ingresando en que hayas ingresado.</t>
+  </si>
+  <si>
+    <t>3) Guardar la hoja de ruta despues de haber seleccionado la zona y agregado los detalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debe redireccionarte a la pagina show.html donde se muestra la hoja de </t>
+  </si>
+  <si>
+    <t>ruta creada</t>
+  </si>
+  <si>
+    <t>4) Hacer click en Imprimir la hoja de ruta</t>
+  </si>
+  <si>
+    <t>Debe generar como pdf para imprimir la hoja de ruta</t>
+  </si>
+  <si>
+    <t>5) Click en Regresar</t>
+  </si>
+  <si>
+    <t>Debe redireccionar a la pagina de buscar hoja de ruta</t>
+  </si>
+  <si>
+    <t>6) Agregar un codigo de barra ya existente de un producto registrado</t>
+  </si>
+  <si>
+    <t>No debe de aparecer en la lista</t>
+  </si>
+  <si>
+    <t>Debe eliminar el producto de la lista</t>
+  </si>
+  <si>
+    <t>7) Click en eliminar el producto de los detalles de hoja de ruta al estar creando la hoja</t>
+  </si>
+  <si>
+    <t>8) Agregar el producto anteriormente eliminado</t>
+  </si>
+  <si>
+    <t>Debe agregarse a la lista de los detalles</t>
+  </si>
+  <si>
+    <t>9) Agregar el texto "Estos productos son de carácter privado" en el campo comentario</t>
+  </si>
+  <si>
+    <t>Al hacer click sobre imprimir debe aparecer en el pdf a lado del campo OBS:</t>
+  </si>
+  <si>
+    <t>10) Ir a Buscar Hoja de Ruta, buscar una hoja de ruta entre un rango de fechas y cuyo</t>
+  </si>
+  <si>
+    <t>estado sea procesado, e intentar editar</t>
+  </si>
+  <si>
+    <t>El boton edit debe estar desactivado si la hoja de ruta esta procesada</t>
+  </si>
+  <si>
+    <t>11) Buscar una hoja de ruta con estado "En proceso", seleccionar e intentar editar</t>
+  </si>
+  <si>
+    <t>Debe redireccionarte a la interfaz para editar la hoja e ruta con los campos</t>
+  </si>
+  <si>
+    <t>de la hoja de ruta seteadas</t>
+  </si>
+  <si>
+    <t>12) Al editar la hoja de ruta, eliminar alguno de sus productos y guardar</t>
+  </si>
+  <si>
+    <t>Esto productos eliminados deben cambiar su estado de "Enviado" a</t>
+  </si>
+  <si>
+    <t>"No Enviado", y la hoja de ruta ahora debe aparecer sin estos productos</t>
+  </si>
+  <si>
+    <t>Hoja de Ruta(Tener en cuenta el orden de los productos que se van registrando. El primero</t>
+  </si>
+  <si>
+    <t>debe estar en la primera posicion, el segundo en el segundo y asi….)</t>
+  </si>
+  <si>
+    <t>Programador: Wildo Monges</t>
+  </si>
+  <si>
+    <t>Tester: Leois linka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -854,6 +959,14 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -876,12 +989,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,7 +1006,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1176,13 +1290,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="81.85546875" customWidth="1"/>
@@ -2391,6 +2505,156 @@
     <row r="191" spans="1:3">
       <c r="C191" t="s">
         <v>269</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="B194" t="s">
+        <v>304</v>
+      </c>
+      <c r="C194" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="B196" t="s">
+        <v>271</v>
+      </c>
+      <c r="C196" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="C197" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="C198" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="B200" t="s">
+        <v>275</v>
+      </c>
+      <c r="C200" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="C201" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="B203" t="s">
+        <v>278</v>
+      </c>
+      <c r="C203" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="C204" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="B205" t="s">
+        <v>281</v>
+      </c>
+      <c r="C205" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="B207" t="s">
+        <v>283</v>
+      </c>
+      <c r="C207" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3">
+      <c r="B209" t="s">
+        <v>285</v>
+      </c>
+      <c r="C209" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3">
+      <c r="B210" t="s">
+        <v>288</v>
+      </c>
+      <c r="C210" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3">
+      <c r="B211" t="s">
+        <v>289</v>
+      </c>
+      <c r="C211" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3">
+      <c r="B212" t="s">
+        <v>291</v>
+      </c>
+      <c r="C212" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3">
+      <c r="B213" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3">
+      <c r="B214" t="s">
+        <v>294</v>
+      </c>
+      <c r="C214" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3">
+      <c r="B215" t="s">
+        <v>296</v>
+      </c>
+      <c r="C215" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3">
+      <c r="C216" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3">
+      <c r="B217" t="s">
+        <v>299</v>
+      </c>
+      <c r="C217" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3">
+      <c r="C218" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2408,7 +2672,7 @@
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
@@ -3298,7 +3562,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizando plan de testeo con resultados
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21255" windowHeight="9975"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20730" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Wildo" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="286">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -829,6 +829,51 @@
   </si>
   <si>
     <t>Roles y Permisos</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Muestra el mensaje, no guarda la nota</t>
+  </si>
+  <si>
+    <t>Muestra el mensaje, se guarda la nota</t>
+  </si>
+  <si>
+    <t>Muestra el mensaje, se actualiza la nota</t>
+  </si>
+  <si>
+    <t>Muestra el mensaje, no se actualiza</t>
+  </si>
+  <si>
+    <t>Mejorar mensaje de error, en uno aparece cerc en vez de cero</t>
+  </si>
+  <si>
+    <t>Muestra un mensaje, no se actualiza</t>
+  </si>
+  <si>
+    <t>Muestra la nota con todos los datos</t>
+  </si>
+  <si>
+    <t>Elimina la nota de retiro y muestra el mensaje.</t>
+  </si>
+  <si>
+    <t>No elimina la nota de retiro y muestra el mensaje.</t>
+  </si>
+  <si>
+    <t>Verificado</t>
+  </si>
+  <si>
+    <t>Verificado. No veo el sentido de cambiar a procesado</t>
+  </si>
+  <si>
+    <t>Al ingresar un numero de nota ya procesada, al hacer click en guardar, muestra en la nota en la tabla</t>
+  </si>
+  <si>
+    <t>Permitir el usuario editar el estado de la nota de retiro solo a cancelado o perdido</t>
+  </si>
+  <si>
+    <t>Al crear una nueva nota de retiro, guarda la nota al seleccionar una fecha de vencimiento menor a la fecha de retiro.</t>
   </si>
 </sst>
 </file>
@@ -1176,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1382,7 +1427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>9</v>
       </c>
@@ -1393,7 +1438,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -1401,7 +1446,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1411,8 +1456,11 @@
       <c r="C38" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1422,8 +1470,11 @@
       <c r="C39" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1433,8 +1484,11 @@
       <c r="C40" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1444,8 +1498,11 @@
       <c r="C41" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1455,8 +1512,11 @@
       <c r="C42" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>6</v>
       </c>
@@ -1466,21 +1526,30 @@
       <c r="C43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D43" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="B45" t="s">
         <v>53</v>
       </c>
       <c r="C45" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="C46" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>7</v>
       </c>
@@ -1490,8 +1559,11 @@
       <c r="C47" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>8</v>
       </c>
@@ -1501,8 +1573,11 @@
       <c r="C48" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>9</v>
       </c>
@@ -1512,13 +1587,19 @@
       <c r="C49" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="C50" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>10</v>
       </c>
@@ -1528,21 +1609,30 @@
       <c r="C51" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="C52" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>11</v>
       </c>
       <c r="B53" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>12</v>
       </c>
@@ -1552,8 +1642,11 @@
       <c r="C54" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>13</v>
       </c>
@@ -1563,222 +1656,106 @@
       <c r="C55" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D55" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>14</v>
       </c>
       <c r="B57" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1" t="s">
+      <c r="D57" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>271</v>
+      </c>
+      <c r="D58" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="D59" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60">
+    <row r="76" spans="1:3">
+      <c r="A76">
         <v>1</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B76" t="s">
         <v>77</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C76" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61">
-        <v>2</v>
-      </c>
-      <c r="B61" t="s">
-        <v>74</v>
-      </c>
-      <c r="C61" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62">
-        <v>3</v>
-      </c>
-      <c r="B62" t="s">
-        <v>80</v>
-      </c>
-      <c r="C62" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63">
-        <v>4</v>
-      </c>
-      <c r="B63" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64">
-        <v>5</v>
-      </c>
-      <c r="B64" t="s">
-        <v>82</v>
-      </c>
-      <c r="C64" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65">
-        <v>6</v>
-      </c>
-      <c r="B65" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66">
-        <v>7</v>
-      </c>
-      <c r="B66" t="s">
-        <v>148</v>
-      </c>
-      <c r="C66" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67">
-        <v>8</v>
-      </c>
-      <c r="B67" t="s">
-        <v>150</v>
-      </c>
-      <c r="C67" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68">
-        <v>9</v>
-      </c>
-      <c r="B68" t="s">
-        <v>152</v>
-      </c>
-      <c r="C68" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
-        <v>154</v>
-      </c>
-      <c r="C69" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72">
-        <v>1</v>
-      </c>
-      <c r="B72" t="s">
-        <v>157</v>
-      </c>
-      <c r="C72" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="C73" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74">
-        <v>2</v>
-      </c>
-      <c r="B74" t="s">
-        <v>160</v>
-      </c>
-      <c r="C74" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75">
-        <v>3</v>
-      </c>
-      <c r="B75" t="s">
-        <v>162</v>
-      </c>
-      <c r="C75" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="C76" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>168</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:3">
+      <c r="A79">
+        <v>4</v>
+      </c>
       <c r="B79" t="s">
-        <v>167</v>
+        <v>75</v>
+      </c>
+      <c r="C79" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>82</v>
+      </c>
+      <c r="C80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
         <v>6</v>
       </c>
-      <c r="B80" t="s">
-        <v>170</v>
-      </c>
-      <c r="C80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="C81" t="s">
-        <v>172</v>
+      <c r="B81" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1786,7 +1763,10 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>173</v>
+        <v>148</v>
+      </c>
+      <c r="C82" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1794,602 +1774,737 @@
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>174</v>
+        <v>150</v>
+      </c>
+      <c r="C83" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:3">
+      <c r="A84">
+        <v>9</v>
+      </c>
       <c r="B84" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="C84" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86">
-        <v>9</v>
-      </c>
-      <c r="B86" t="s">
-        <v>178</v>
-      </c>
-      <c r="C86" t="s">
-        <v>177</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s">
+        <v>154</v>
+      </c>
+      <c r="C85" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87">
-        <v>10</v>
-      </c>
-      <c r="B87" t="s">
-        <v>179</v>
-      </c>
-      <c r="C87" t="s">
-        <v>180</v>
+      <c r="A87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="C88" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="C89" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="C90" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="C91" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92">
-        <v>14</v>
-      </c>
-      <c r="B92" t="s">
-        <v>188</v>
+      <c r="C92" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="C93" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
+        <v>5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>169</v>
+      </c>
+      <c r="C94" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="B95" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>6</v>
+      </c>
+      <c r="B96" t="s">
+        <v>170</v>
+      </c>
+      <c r="C96" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="C97" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>7</v>
+      </c>
+      <c r="B98" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>8</v>
+      </c>
+      <c r="B99" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="B100" t="s">
+        <v>175</v>
+      </c>
+      <c r="C100" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102">
+        <v>9</v>
+      </c>
+      <c r="B102" t="s">
+        <v>178</v>
+      </c>
+      <c r="C102" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103">
+        <v>10</v>
+      </c>
+      <c r="B103" t="s">
+        <v>179</v>
+      </c>
+      <c r="C103" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104">
+        <v>11</v>
+      </c>
+      <c r="B104" t="s">
+        <v>182</v>
+      </c>
+      <c r="C104" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="C105" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106">
+        <v>12</v>
+      </c>
+      <c r="B106" t="s">
+        <v>184</v>
+      </c>
+      <c r="C106" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>13</v>
+      </c>
+      <c r="B107" t="s">
+        <v>186</v>
+      </c>
+      <c r="C107" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109">
+        <v>15</v>
+      </c>
+      <c r="B109" t="s">
+        <v>189</v>
+      </c>
+      <c r="C109" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110">
         <v>16</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B110" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="1" t="s">
+    <row r="113" spans="1:4">
+      <c r="A113" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B113" t="s">
         <v>193</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="1" t="s">
+    <row r="114" spans="1:4">
+      <c r="A114" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="B99" s="1" t="s">
+    <row r="115" spans="1:4">
+      <c r="B115" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D115" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100">
+    <row r="116" spans="1:4">
+      <c r="A116">
         <v>1</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B116" t="s">
         <v>194</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C116" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="C101" t="s">
+    <row r="117" spans="1:4">
+      <c r="C117" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103">
+    <row r="119" spans="1:4">
+      <c r="A119">
         <v>2</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B119" t="s">
         <v>12</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C119" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="C104" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106">
-        <v>3</v>
-      </c>
-      <c r="B106" t="s">
-        <v>196</v>
-      </c>
-      <c r="C106" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="C107" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110">
-        <v>4</v>
-      </c>
-      <c r="B110" t="s">
-        <v>198</v>
-      </c>
-      <c r="C110" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="C111" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113">
-        <v>5</v>
-      </c>
-      <c r="B113" t="s">
-        <v>202</v>
-      </c>
-      <c r="C113" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115">
-        <v>6</v>
-      </c>
-      <c r="B115" t="s">
-        <v>203</v>
-      </c>
-      <c r="C115" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="C116" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118">
-        <v>7</v>
-      </c>
-      <c r="B118" t="s">
-        <v>26</v>
-      </c>
-      <c r="C118" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="C119" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="C120" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="C121" t="s">
-        <v>208</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:4">
+      <c r="A122">
+        <v>3</v>
+      </c>
+      <c r="B122" t="s">
+        <v>196</v>
+      </c>
       <c r="C122" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="C123" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126">
+        <v>4</v>
+      </c>
+      <c r="B126" t="s">
+        <v>198</v>
+      </c>
+      <c r="C126" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="C127" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129">
+        <v>5</v>
+      </c>
+      <c r="B129" t="s">
+        <v>202</v>
+      </c>
+      <c r="C129" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131">
+        <v>6</v>
+      </c>
+      <c r="B131" t="s">
+        <v>203</v>
+      </c>
+      <c r="C131" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="C132" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134">
+        <v>7</v>
+      </c>
+      <c r="B134" t="s">
+        <v>26</v>
+      </c>
+      <c r="C134" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="C135" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="C136" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="C137" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="C138" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="C139" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="1" t="s">
+    <row r="141" spans="1:4">
+      <c r="A141" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
-      <c r="B126" s="1" t="s">
+    <row r="142" spans="1:4">
+      <c r="B142" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C142" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D142" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
-      <c r="A127">
+    <row r="143" spans="1:4">
+      <c r="A143">
         <v>1</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B143" t="s">
         <v>213</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C143" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
-      <c r="C128" t="s">
+    <row r="144" spans="1:4">
+      <c r="C144" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
-      <c r="A130">
+    <row r="146" spans="1:3">
+      <c r="A146">
         <v>2</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B146" t="s">
         <v>216</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C146" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
-      <c r="C131" t="s">
+    <row r="147" spans="1:3">
+      <c r="C147" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
-      <c r="A133">
+    <row r="149" spans="1:3">
+      <c r="A149">
         <v>3</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B149" t="s">
         <v>219</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C149" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
-      <c r="A140">
+    <row r="156" spans="1:3">
+      <c r="A156">
         <v>4</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B156" t="s">
         <v>222</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C156" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
-      <c r="A142">
+    <row r="158" spans="1:3">
+      <c r="A158">
         <v>5</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B158" t="s">
         <v>224</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C158" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
-      <c r="C143" t="s">
+    <row r="159" spans="1:3">
+      <c r="C159" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
-      <c r="A145">
+    <row r="161" spans="1:4">
+      <c r="A161">
         <v>6</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B161" t="s">
         <v>26</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C161" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
-      <c r="C146" t="s">
+    <row r="162" spans="1:4">
+      <c r="C162" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
-      <c r="C147" t="s">
+    <row r="163" spans="1:4">
+      <c r="C163" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
-      <c r="C148" t="s">
+    <row r="164" spans="1:4">
+      <c r="C164" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
-      <c r="C149" t="s">
+    <row r="165" spans="1:4">
+      <c r="C165" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
-      <c r="A151" s="1" t="s">
+    <row r="167" spans="1:4">
+      <c r="A167" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B167" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
-      <c r="B152" s="1" t="s">
+    <row r="168" spans="1:4">
+      <c r="B168" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C168" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D168" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
-      <c r="A153">
+    <row r="169" spans="1:4">
+      <c r="A169">
         <v>1</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B169" t="s">
         <v>231</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C169" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
-      <c r="C154" t="s">
+    <row r="170" spans="1:4">
+      <c r="C170" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
-      <c r="A156">
+    <row r="172" spans="1:4">
+      <c r="A172">
         <v>2</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B172" t="s">
         <v>263</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C172" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
-      <c r="A158">
+    <row r="174" spans="1:4">
+      <c r="A174">
         <v>3</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B174" t="s">
         <v>234</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C174" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
-      <c r="B159" t="s">
+    <row r="175" spans="1:4">
+      <c r="B175" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
-      <c r="B160" t="s">
+    <row r="176" spans="1:4">
+      <c r="B176" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="161" spans="2:2">
-      <c r="B161" t="s">
+    <row r="177" spans="2:2">
+      <c r="B177" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="162" spans="2:2">
-      <c r="B162" t="s">
+    <row r="178" spans="2:2">
+      <c r="B178" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="163" spans="2:2">
-      <c r="B163" t="s">
+    <row r="179" spans="2:2">
+      <c r="B179" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="164" spans="2:2">
-      <c r="B164" t="s">
+    <row r="180" spans="2:2">
+      <c r="B180" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="165" spans="2:2">
-      <c r="B165" t="s">
+    <row r="181" spans="2:2">
+      <c r="B181" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="166" spans="2:2">
-      <c r="B166" t="s">
+    <row r="182" spans="2:2">
+      <c r="B182" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="167" spans="2:2">
-      <c r="B167" t="s">
+    <row r="183" spans="2:2">
+      <c r="B183" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="168" spans="2:2">
-      <c r="B168" t="s">
+    <row r="184" spans="2:2">
+      <c r="B184" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="169" spans="2:2">
-      <c r="B169" t="s">
+    <row r="185" spans="2:2">
+      <c r="B185" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="170" spans="2:2">
-      <c r="B170" t="s">
+    <row r="186" spans="2:2">
+      <c r="B186" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="171" spans="2:2">
-      <c r="B171" t="s">
+    <row r="187" spans="2:2">
+      <c r="B187" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="172" spans="2:2">
-      <c r="B172" t="s">
+    <row r="188" spans="2:2">
+      <c r="B188" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="173" spans="2:2">
-      <c r="B173" t="s">
+    <row r="189" spans="2:2">
+      <c r="B189" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="174" spans="2:2">
-      <c r="B174" t="s">
+    <row r="190" spans="2:2">
+      <c r="B190" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="175" spans="2:2">
-      <c r="B175" t="s">
+    <row r="191" spans="2:2">
+      <c r="B191" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="176" spans="2:2">
-      <c r="B176" t="s">
+    <row r="192" spans="2:2">
+      <c r="B192" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
-      <c r="B177" t="s">
+    <row r="193" spans="1:3">
+      <c r="B193" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
-      <c r="B178" t="s">
+    <row r="194" spans="1:3">
+      <c r="B194" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
-      <c r="B179" t="s">
+    <row r="195" spans="1:3">
+      <c r="B195" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
-      <c r="B180" t="s">
+    <row r="196" spans="1:3">
+      <c r="B196" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
-      <c r="B181" t="s">
+    <row r="197" spans="1:3">
+      <c r="B197" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
-      <c r="B182" t="s">
+    <row r="198" spans="1:3">
+      <c r="B198" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
-      <c r="A184">
+    <row r="200" spans="1:3">
+      <c r="A200">
         <v>4</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B200" t="s">
         <v>259</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C200" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
-      <c r="B185" t="s">
+    <row r="201" spans="1:3">
+      <c r="B201" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
-      <c r="B186" t="s">
+    <row r="202" spans="1:3">
+      <c r="B202" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
-      <c r="B187" t="s">
+    <row r="203" spans="1:3">
+      <c r="B203" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
-      <c r="A189">
+    <row r="205" spans="1:3">
+      <c r="A205">
         <v>5</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B205" t="s">
         <v>266</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C205" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
-      <c r="C190" t="s">
+    <row r="206" spans="1:3">
+      <c r="C206" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
-      <c r="C191" t="s">
+    <row r="207" spans="1:3">
+      <c r="C207" t="s">
         <v>269</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizar plan de testeo con los issues creados por los bugs encontrados
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="287">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -874,6 +874,9 @@
   </si>
   <si>
     <t>Al crear una nueva nota de retiro, guarda la nota al seleccionar una fecha de vencimiento menor a la fecha de retiro.</t>
+  </si>
+  <si>
+    <t>Quitar el estado perdido de las notas de retiro, no hace falta, con cancelar es suficiente</t>
   </si>
 </sst>
 </file>
@@ -1221,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="C39" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1577,7 +1580,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>9</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="C50" t="s">
         <v>62</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>10</v>
       </c>
@@ -1613,15 +1616,18 @@
         <v>282</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="C52" t="s">
         <v>65</v>
       </c>
       <c r="D52" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>11</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>12</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>13</v>
       </c>
@@ -1660,7 +1666,15 @@
         <v>281</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="56" spans="1:5">
+      <c r="D56" t="s">
+        <v>286</v>
+      </c>
+      <c r="E56">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>14</v>
       </c>
@@ -1670,8 +1684,11 @@
       <c r="D57" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>15</v>
       </c>
@@ -1682,9 +1699,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="D59" t="s">
         <v>285</v>
+      </c>
+      <c r="E59">
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:3">

</xml_diff>

<commit_message>
actualizacion de plan de testeo, agregar issues a los bugs encontrados (149)
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="290">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -877,13 +877,22 @@
   </si>
   <si>
     <t>Quitar el estado perdido de las notas de retiro, no hace falta, con cancelar es suficiente</t>
+  </si>
+  <si>
+    <t>Permite guardar una nota de retiro con cantidad 0 (validacion)</t>
+  </si>
+  <si>
+    <t>Al hacer click en limpiar se borra el campo funcionario (creo que no es necesario ese campo)</t>
+  </si>
+  <si>
+    <t>Actualmente se puede agregar a una hoja de ruta productos pertenecientes a una nota de retiro cancelada (pasos: crear una nota de retiro con 5 productos, registrar 3 productos, cancelar la nota de retiro, agregar a una hoja de ruta los 3 productos registrados, creo que hay necesidad de definir eso con el cliente)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,6 +910,12 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="63"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -924,12 +939,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1224,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E207"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C39" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1667,864 +1683,882 @@
       </c>
     </row>
     <row r="56" spans="1:5">
+      <c r="A56">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>271</v>
+      </c>
       <c r="D56" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E56">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57">
-        <v>14</v>
-      </c>
-      <c r="B57" t="s">
-        <v>71</v>
-      </c>
-      <c r="D57" t="s">
-        <v>284</v>
+      <c r="D57" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="E57">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58">
-        <v>15</v>
-      </c>
-      <c r="B58" t="s">
-        <v>271</v>
-      </c>
-      <c r="D58" t="s">
-        <v>276</v>
+      <c r="D58" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E58">
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="D59" t="s">
+        <v>286</v>
+      </c>
+      <c r="E59">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="D60" t="s">
+        <v>284</v>
+      </c>
+      <c r="E60">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="D61" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="D62" t="s">
         <v>285</v>
       </c>
-      <c r="E59">
+      <c r="E62">
         <v>157</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76">
-        <v>1</v>
-      </c>
-      <c r="B76" t="s">
-        <v>77</v>
-      </c>
-      <c r="C76" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77">
-        <v>2</v>
-      </c>
-      <c r="B77" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78">
-        <v>3</v>
-      </c>
-      <c r="B78" t="s">
-        <v>80</v>
-      </c>
-      <c r="C78" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="C81" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="C82" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>151</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>152</v>
-      </c>
-      <c r="C84" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C85" t="s">
-        <v>155</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>8</v>
+      </c>
+      <c r="B86" t="s">
+        <v>150</v>
+      </c>
+      <c r="C86" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>156</v>
+      <c r="A87">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>152</v>
+      </c>
+      <c r="C87" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
+        <v>10</v>
+      </c>
+      <c r="B88" t="s">
+        <v>154</v>
+      </c>
+      <c r="C88" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B88" t="s">
-        <v>157</v>
-      </c>
-      <c r="C88" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="C89" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90">
-        <v>2</v>
-      </c>
-      <c r="B90" t="s">
-        <v>160</v>
-      </c>
-      <c r="C90" t="s">
-        <v>161</v>
+      <c r="B90" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C91" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="C92" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C93" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C94" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="B95" t="s">
-        <v>167</v>
+      <c r="C95" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B96" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C96" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:3">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>169</v>
+      </c>
       <c r="C97" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98">
-        <v>7</v>
-      </c>
       <c r="B98" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B99" t="s">
-        <v>174</v>
+        <v>170</v>
+      </c>
+      <c r="C99" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="B100" t="s">
-        <v>175</v>
-      </c>
       <c r="C100" t="s">
-        <v>176</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101">
+        <v>7</v>
+      </c>
+      <c r="B101" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102">
+        <v>8</v>
+      </c>
+      <c r="B102" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="B103" t="s">
+        <v>175</v>
+      </c>
+      <c r="C103" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
         <v>9</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B105" t="s">
         <v>178</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C105" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103">
-        <v>10</v>
-      </c>
-      <c r="B103" t="s">
-        <v>179</v>
-      </c>
-      <c r="C103" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104">
-        <v>11</v>
-      </c>
-      <c r="B104" t="s">
-        <v>182</v>
-      </c>
-      <c r="C104" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="C105" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C106" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C107" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108">
-        <v>14</v>
-      </c>
-      <c r="B108" t="s">
-        <v>188</v>
+      <c r="C108" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B109" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C109" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110">
+        <v>13</v>
+      </c>
+      <c r="B110" t="s">
+        <v>186</v>
+      </c>
+      <c r="C110" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111">
+        <v>14</v>
+      </c>
+      <c r="B111" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112">
+        <v>15</v>
+      </c>
+      <c r="B112" t="s">
+        <v>189</v>
+      </c>
+      <c r="C112" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113">
         <v>16</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B113" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="1" t="s">
+    <row r="116" spans="1:4">
+      <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B116" t="s">
         <v>193</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C116" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="1" t="s">
+    <row r="117" spans="1:4">
+      <c r="A117" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
-      <c r="B115" s="1" t="s">
+    <row r="118" spans="1:4">
+      <c r="B118" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D118" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116">
-        <v>1</v>
-      </c>
-      <c r="B116" t="s">
-        <v>194</v>
-      </c>
-      <c r="C116" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="C117" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>12</v>
+        <v>194</v>
       </c>
       <c r="C119" t="s">
-        <v>13</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="C120" t="s">
-        <v>14</v>
+        <v>195</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B122" t="s">
-        <v>196</v>
+        <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>220</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="C123" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125">
+        <v>3</v>
+      </c>
+      <c r="B125" t="s">
+        <v>196</v>
+      </c>
+      <c r="C125" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="C126" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
-      <c r="A126">
+    <row r="129" spans="1:3">
+      <c r="A129">
         <v>4</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B129" t="s">
         <v>198</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C129" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
-      <c r="C127" t="s">
+    <row r="130" spans="1:3">
+      <c r="C130" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129">
+    <row r="132" spans="1:3">
+      <c r="A132">
         <v>5</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B132" t="s">
         <v>202</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C132" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
-      <c r="A131">
+    <row r="134" spans="1:3">
+      <c r="A134">
         <v>6</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B134" t="s">
         <v>203</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C134" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
-      <c r="C132" t="s">
+    <row r="135" spans="1:3">
+      <c r="C135" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
-      <c r="A134">
+    <row r="137" spans="1:3">
+      <c r="A137">
         <v>7</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B137" t="s">
         <v>26</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C137" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
-      <c r="C135" t="s">
+    <row r="138" spans="1:3">
+      <c r="C138" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="C136" t="s">
+    <row r="139" spans="1:3">
+      <c r="C139" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
-      <c r="C137" t="s">
+    <row r="140" spans="1:3">
+      <c r="C140" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
-      <c r="C138" t="s">
+    <row r="141" spans="1:3">
+      <c r="C141" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
-      <c r="C139" t="s">
+    <row r="142" spans="1:3">
+      <c r="C142" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="1" t="s">
+    <row r="144" spans="1:3">
+      <c r="A144" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B144" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
-      <c r="B142" s="1" t="s">
+    <row r="145" spans="1:4">
+      <c r="B145" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C145" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D145" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
-      <c r="A143">
+    <row r="146" spans="1:4">
+      <c r="A146">
         <v>1</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B146" t="s">
         <v>213</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C146" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
-      <c r="C144" t="s">
+    <row r="147" spans="1:4">
+      <c r="C147" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
-      <c r="A146">
+    <row r="149" spans="1:4">
+      <c r="A149">
         <v>2</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B149" t="s">
         <v>216</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C149" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
-      <c r="C147" t="s">
+    <row r="150" spans="1:4">
+      <c r="C150" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
-      <c r="A149">
+    <row r="152" spans="1:4">
+      <c r="A152">
         <v>3</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B152" t="s">
         <v>219</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C152" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
-      <c r="A156">
+    <row r="159" spans="1:4">
+      <c r="A159">
         <v>4</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B159" t="s">
         <v>222</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C159" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158">
-        <v>5</v>
-      </c>
-      <c r="B158" t="s">
-        <v>224</v>
-      </c>
-      <c r="C158" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="C159" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B161" t="s">
-        <v>26</v>
+        <v>224</v>
       </c>
       <c r="C161" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="C162" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
-      <c r="C163" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="164" spans="1:4">
+      <c r="A164">
+        <v>6</v>
+      </c>
+      <c r="B164" t="s">
+        <v>26</v>
+      </c>
       <c r="C164" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="C165" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="C166" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="C167" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="C168" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
-      <c r="A167" s="1" t="s">
+    <row r="170" spans="1:4">
+      <c r="A170" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B170" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
-      <c r="B168" s="1" t="s">
+    <row r="171" spans="1:4">
+      <c r="B171" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="C171" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D171" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
-      <c r="A169">
-        <v>1</v>
-      </c>
-      <c r="B169" t="s">
-        <v>231</v>
-      </c>
-      <c r="C169" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
-      <c r="C170" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172">
+        <v>1</v>
+      </c>
+      <c r="B172" t="s">
+        <v>231</v>
+      </c>
+      <c r="C172" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="C173" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175">
         <v>2</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B175" t="s">
         <v>263</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C175" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
-      <c r="A174">
+    <row r="177" spans="1:3">
+      <c r="A177">
         <v>3</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B177" t="s">
         <v>234</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C177" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
-      <c r="B175" t="s">
+    <row r="178" spans="1:3">
+      <c r="B178" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
-      <c r="B176" t="s">
+    <row r="179" spans="1:3">
+      <c r="B179" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="177" spans="2:2">
-      <c r="B177" t="s">
+    <row r="180" spans="1:3">
+      <c r="B180" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="178" spans="2:2">
-      <c r="B178" t="s">
+    <row r="181" spans="1:3">
+      <c r="B181" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="179" spans="2:2">
-      <c r="B179" t="s">
+    <row r="182" spans="1:3">
+      <c r="B182" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="180" spans="2:2">
-      <c r="B180" t="s">
+    <row r="183" spans="1:3">
+      <c r="B183" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="181" spans="2:2">
-      <c r="B181" t="s">
+    <row r="184" spans="1:3">
+      <c r="B184" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="182" spans="2:2">
-      <c r="B182" t="s">
+    <row r="185" spans="1:3">
+      <c r="B185" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="183" spans="2:2">
-      <c r="B183" t="s">
+    <row r="186" spans="1:3">
+      <c r="B186" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="2:2">
-      <c r="B184" t="s">
+    <row r="187" spans="1:3">
+      <c r="B187" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="185" spans="2:2">
-      <c r="B185" t="s">
+    <row r="188" spans="1:3">
+      <c r="B188" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="2:2">
-      <c r="B186" t="s">
+    <row r="189" spans="1:3">
+      <c r="B189" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="2:2">
-      <c r="B187" t="s">
+    <row r="190" spans="1:3">
+      <c r="B190" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="188" spans="2:2">
-      <c r="B188" t="s">
+    <row r="191" spans="1:3">
+      <c r="B191" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="2:2">
-      <c r="B189" t="s">
+    <row r="192" spans="1:3">
+      <c r="B192" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="190" spans="2:2">
-      <c r="B190" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="191" spans="2:2">
-      <c r="B191" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="192" spans="2:2">
-      <c r="B192" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="B193" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="B194" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="B195" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="B196" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="B197" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="B198" t="s">
-        <v>257</v>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="B199" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200">
-        <v>4</v>
-      </c>
       <c r="B200" t="s">
-        <v>259</v>
-      </c>
-      <c r="C200" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="B201" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203">
+        <v>4</v>
+      </c>
+      <c r="B203" t="s">
+        <v>259</v>
+      </c>
+      <c r="C203" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="B204" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
-      <c r="B202" t="s">
+    <row r="205" spans="1:3">
+      <c r="B205" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
-      <c r="B203" t="s">
+    <row r="206" spans="1:3">
+      <c r="B206" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
-      <c r="A205">
+    <row r="208" spans="1:3">
+      <c r="A208">
         <v>5</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B208" t="s">
         <v>266</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C208" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
-      <c r="C206" t="s">
+    <row r="209" spans="3:3">
+      <c r="C209" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
-      <c r="C207" t="s">
+    <row r="210" spans="3:3">
+      <c r="C210" t="s">
         <v>269</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualización del plan de testeo
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="307">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -591,9 +591,6 @@
     <t>El producto debe eliminarse de la lista y de la bd. El item debe disminuir en 1</t>
   </si>
   <si>
-    <t>Aplicar tus propias formas de testear</t>
-  </si>
-  <si>
     <t>Destinatarios</t>
   </si>
   <si>
@@ -886,6 +883,60 @@
   </si>
   <si>
     <t>Actualmente se puede agregar a una hoja de ruta productos pertenecientes a una nota de retiro cancelada (pasos: crear una nota de retiro con 5 productos, registrar 3 productos, cancelar la nota de retiro, agregar a una hoja de ruta los 3 productos registrados, creo que hay necesidad de definir eso con el cliente)</t>
+  </si>
+  <si>
+    <t>Verificado, aparece el numero de la nota de retiro en el autocomplete.</t>
+  </si>
+  <si>
+    <t>Aparecen los destinatarios al ingresar "2" letras en el autocomplete.</t>
+  </si>
+  <si>
+    <t>Modificar fecha</t>
+  </si>
+  <si>
+    <t>Al modificar la fecha no guarda el producto</t>
+  </si>
+  <si>
+    <t>Verificado, al seleccionar el focus va sobre código de barras</t>
+  </si>
+  <si>
+    <t>No verificado</t>
+  </si>
+  <si>
+    <t>Verificado, no se puede guardar mas que "Cantidad Productos" productos</t>
+  </si>
+  <si>
+    <t>Verificado, aparece los productos registrados anteriormente.</t>
+  </si>
+  <si>
+    <t>Verificado, es posible registrar un nuevo destinatario y luego usarlo</t>
+  </si>
+  <si>
+    <t>Verificado.</t>
+  </si>
+  <si>
+    <t>Verificado, se guardan correctamente.</t>
+  </si>
+  <si>
+    <t>Verificado, no permite ingresar 2 codigos de barra iguales</t>
+  </si>
+  <si>
+    <t>Verificado, se comporta como esperado.</t>
+  </si>
+  <si>
+    <t>Al seleccionar la dirección "seleccionar", hacer click</t>
+  </si>
+  <si>
+    <t>y hacer click en guardar</t>
+  </si>
+  <si>
+    <t>Deberia guardar el producto al tener una direccion valida</t>
+  </si>
+  <si>
+    <t>en guardar, luego intentar seleccionar una dirección valida</t>
+  </si>
+  <si>
+    <t>No guarda el producto.</t>
   </si>
 </sst>
 </file>
@@ -1242,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C39" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="C90" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1476,7 +1527,7 @@
         <v>42</v>
       </c>
       <c r="D38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1490,7 +1541,7 @@
         <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1504,7 +1555,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1518,7 +1569,7 @@
         <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1532,7 +1583,7 @@
         <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1546,7 +1597,7 @@
         <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1557,7 +1608,7 @@
         <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1565,7 +1616,7 @@
         <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1579,7 +1630,7 @@
         <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1593,7 +1644,7 @@
         <v>59</v>
       </c>
       <c r="D48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1607,7 +1658,7 @@
         <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1615,7 +1666,7 @@
         <v>62</v>
       </c>
       <c r="D50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1629,7 +1680,7 @@
         <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1637,7 +1688,7 @@
         <v>65</v>
       </c>
       <c r="D52" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E52">
         <v>158</v>
@@ -1651,7 +1702,7 @@
         <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1665,7 +1716,7 @@
         <v>68</v>
       </c>
       <c r="D54" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1679,7 +1730,7 @@
         <v>70</v>
       </c>
       <c r="D55" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1687,10 +1738,10 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D56" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E56">
         <v>149</v>
@@ -1698,7 +1749,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="D57" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E57">
         <v>149</v>
@@ -1706,7 +1757,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="D58" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E58">
         <v>149</v>
@@ -1714,7 +1765,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="D59" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E59">
         <v>156</v>
@@ -1722,7 +1773,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="D60" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E60">
         <v>159</v>
@@ -1730,12 +1781,12 @@
     </row>
     <row r="61" spans="1:5">
       <c r="D61" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="D62" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E62">
         <v>157</v>
@@ -1771,7 +1822,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>3</v>
       </c>
@@ -1782,7 +1833,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>4</v>
       </c>
@@ -1793,7 +1844,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>5</v>
       </c>
@@ -1804,7 +1855,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>6</v>
       </c>
@@ -1812,7 +1863,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>7</v>
       </c>
@@ -1823,7 +1874,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>8</v>
       </c>
@@ -1834,7 +1885,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>9</v>
       </c>
@@ -1845,7 +1896,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>10</v>
       </c>
@@ -1856,7 +1907,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
         <v>1</v>
       </c>
@@ -1864,7 +1915,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>1</v>
       </c>
@@ -1874,13 +1925,16 @@
       <c r="C91" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="D91" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="C92" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>2</v>
       </c>
@@ -1890,8 +1944,14 @@
       <c r="C93" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="D93" t="s">
+        <v>290</v>
+      </c>
+      <c r="E93">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>3</v>
       </c>
@@ -1901,13 +1961,16 @@
       <c r="C94" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="D94" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="C95" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>4</v>
       </c>
@@ -1917,8 +1980,11 @@
       <c r="C96" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>5</v>
       </c>
@@ -1928,13 +1994,16 @@
       <c r="C97" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="B98" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>6</v>
       </c>
@@ -1944,37 +2013,49 @@
       <c r="C99" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="D99" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="C100" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>7</v>
       </c>
       <c r="B101" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="D101" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102">
         <v>8</v>
       </c>
       <c r="B102" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="D102" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="B103" t="s">
         <v>175</v>
       </c>
       <c r="C103" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="D103" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105">
         <v>9</v>
       </c>
@@ -1984,8 +2065,11 @@
       <c r="C105" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="D105" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106">
         <v>10</v>
       </c>
@@ -1995,8 +2079,11 @@
       <c r="C106" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="D106" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107">
         <v>11</v>
       </c>
@@ -2006,13 +2093,16 @@
       <c r="C107" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="D107" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="C108" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:4">
       <c r="A109">
         <v>12</v>
       </c>
@@ -2022,8 +2112,11 @@
       <c r="C109" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="D109" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110">
         <v>13</v>
       </c>
@@ -2033,16 +2126,22 @@
       <c r="C110" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="D110" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111">
         <v>14</v>
       </c>
       <c r="B111" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="D111" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112">
         <v>15</v>
       </c>
@@ -2052,37 +2151,68 @@
       <c r="C112" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="D112" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>16</v>
       </c>
       <c r="B113" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
+        <v>270</v>
+      </c>
+      <c r="C113" t="s">
+        <v>291</v>
+      </c>
+      <c r="D113" t="s">
+        <v>292</v>
+      </c>
+      <c r="E113">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="B114" t="s">
+        <v>304</v>
+      </c>
+      <c r="C114" t="s">
+        <v>302</v>
+      </c>
+      <c r="D114" t="s">
+        <v>306</v>
+      </c>
+      <c r="E114">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="C115" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B116" t="s">
-        <v>193</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>192</v>
+      </c>
+      <c r="C116" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="B118" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>3</v>
@@ -2091,23 +2221,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>1</v>
       </c>
       <c r="B119" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="C120" t="s">
         <v>194</v>
       </c>
-      <c r="C119" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="C120" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>2</v>
       </c>
@@ -2118,25 +2248,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:5">
       <c r="C123" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>3</v>
       </c>
       <c r="B125" t="s">
+        <v>195</v>
+      </c>
+      <c r="C125" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="C126" t="s">
         <v>196</v>
-      </c>
-      <c r="C125" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="C126" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2144,15 +2274,15 @@
         <v>4</v>
       </c>
       <c r="B129" t="s">
+        <v>197</v>
+      </c>
+      <c r="C129" t="s">
         <v>198</v>
-      </c>
-      <c r="C129" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="C130" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2160,10 +2290,10 @@
         <v>5</v>
       </c>
       <c r="B132" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C132" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2171,15 +2301,15 @@
         <v>6</v>
       </c>
       <c r="B134" t="s">
+        <v>202</v>
+      </c>
+      <c r="C134" t="s">
         <v>203</v>
-      </c>
-      <c r="C134" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="C135" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2190,12 +2320,12 @@
         <v>26</v>
       </c>
       <c r="C137" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="C138" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2205,17 +2335,17 @@
     </row>
     <row r="140" spans="1:3">
       <c r="C140" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="C141" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="C142" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2223,12 +2353,12 @@
         <v>1</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="B145" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>3</v>
@@ -2242,15 +2372,15 @@
         <v>1</v>
       </c>
       <c r="B146" t="s">
+        <v>212</v>
+      </c>
+      <c r="C146" t="s">
         <v>213</v>
-      </c>
-      <c r="C146" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="C147" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2258,15 +2388,15 @@
         <v>2</v>
       </c>
       <c r="B149" t="s">
+        <v>215</v>
+      </c>
+      <c r="C149" t="s">
         <v>216</v>
-      </c>
-      <c r="C149" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="C150" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2274,10 +2404,10 @@
         <v>3</v>
       </c>
       <c r="B152" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C152" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2285,10 +2415,10 @@
         <v>4</v>
       </c>
       <c r="B159" t="s">
+        <v>221</v>
+      </c>
+      <c r="C159" t="s">
         <v>222</v>
-      </c>
-      <c r="C159" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2296,15 +2426,15 @@
         <v>5</v>
       </c>
       <c r="B161" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C161" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="C162" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2315,27 +2445,27 @@
         <v>26</v>
       </c>
       <c r="C164" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="C165" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="C166" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="C167" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="C168" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2343,12 +2473,12 @@
         <v>1</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="B171" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>3</v>
@@ -2362,15 +2492,15 @@
         <v>1</v>
       </c>
       <c r="B172" t="s">
+        <v>230</v>
+      </c>
+      <c r="C172" t="s">
         <v>231</v>
-      </c>
-      <c r="C172" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="C173" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2378,10 +2508,10 @@
         <v>2</v>
       </c>
       <c r="B175" t="s">
+        <v>262</v>
+      </c>
+      <c r="C175" t="s">
         <v>263</v>
-      </c>
-      <c r="C175" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2389,130 +2519,130 @@
         <v>3</v>
       </c>
       <c r="B177" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C177" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="B178" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="B179" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="B180" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="B181" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="B182" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="B183" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="B184" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="B185" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="B186" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="B187" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="B188" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="B189" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="B190" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="B191" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="B192" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="B193" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="B194" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="B195" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="B196" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="B197" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="B198" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="B199" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="B200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="B201" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -2520,25 +2650,25 @@
         <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C203" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="B204" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="B205" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="B206" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -2546,20 +2676,20 @@
         <v>5</v>
       </c>
       <c r="B208" t="s">
+        <v>265</v>
+      </c>
+      <c r="C208" t="s">
         <v>266</v>
-      </c>
-      <c r="C208" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="209" spans="3:3">
       <c r="C209" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="210" spans="3:3">
       <c r="C210" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion del plan de testeo, mostrar mensajes al usuario en users
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="291">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -964,6 +964,111 @@
   </si>
   <si>
     <t>Cada 10 minutos debe hacer un timeout, debe pedir al usuario que se loguee luego deve volver a la misma pagina donde se encontraba cuando se expiro la session.</t>
+  </si>
+  <si>
+    <t>Las fechas no deberian ser un campo obligatorio</t>
+  </si>
+  <si>
+    <t>Se debe completar las fechas para poder hacer una busqueda</t>
+  </si>
+  <si>
+    <t>Al realizar un informe para un producto entregado su estado debe cambiar a recibido</t>
+  </si>
+  <si>
+    <t>El estado cambia a pendiente</t>
+  </si>
+  <si>
+    <t>Numero debe ser un autocomplete</t>
+  </si>
+  <si>
+    <t>El usuario debe seleccionar una hoja de ruta para realizar el informe, al seleccionar, debe completar automaticamente el nombre del funcionario, la zona, y habilitar el boton listar productos</t>
+  </si>
+  <si>
+    <t>El usuario no debe ser capaz de ingresar dos motivos,  recibido por y no entregado para un mismo producto</t>
+  </si>
+  <si>
+    <t>Al ingresar algun texto para los campos recibido por debe desabilitar los campos No entregado y rutear y vice versa  correspondientes a la misma fila.</t>
+  </si>
+  <si>
+    <t>Al seleccionar una hoja de ruta y al hacer click en listar productos</t>
+  </si>
+  <si>
+    <t>Se deben listar los productos en la tabla inferior para completar el informe</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modulo: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Empleados</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Programador: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Raul Benitez</t>
+    </r>
+  </si>
+  <si>
+    <t>Tester:</t>
+  </si>
+  <si>
+    <t>Mostrar un Empleado haciendo click en el link/button "Mostrar". Debe redirigirse a la pagina show.html.erb para mostrar el Empleado</t>
+  </si>
+  <si>
+    <t>Intente actualizar una nota sin algun campo obligatorio. En cualquiera de los casos guardar o actualizar si ocurren un error:</t>
+  </si>
+  <si>
+    <t>no se debe actualizar, Debe marcar cual campo falta completar. Error al actualizar, verifique los datos ingresados. Error al guardar, verifique los datos ingresados.</t>
+  </si>
+  <si>
+    <t>Debe mostrar un mensaje: Esta GT no puede ser eliminada. verificar si no desaparece de la lista y de la bd.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modulo: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Guía de transporte</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modulo: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Buscar guía de transporte</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1017,17 +1122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1035,10 +1136,43 @@
       <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1352,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2242,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G165"/>
+  <dimension ref="A1:G230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:IV26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2263,10 +2397,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2276,690 +2410,713 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>245</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>240</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="60">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="45">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>4</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>5</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="30">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>6</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="9">
+      <c r="A15" s="17">
         <v>7</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="7" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="7" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="7" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="9"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="7" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="7" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="9"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="7" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="30">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="7" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="A23" s="5">
+        <v>8</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="7">
-        <v>8</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="A24" s="5">
+        <v>9</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="7">
-        <v>9</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="A27" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="4" t="s">
-        <v>247</v>
-      </c>
+      <c r="A29" s="5"/>
+      <c r="B29" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" t="s">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="5">
+        <v>2</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="5">
+        <v>4</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="5">
+        <v>5</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="30">
+      <c r="A35" s="5">
+        <v>6</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="30">
+      <c r="A36" s="5">
+        <v>7</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="60">
+      <c r="A37" s="5">
+        <v>8</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E37" s="7">
+        <v>158</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" s="5">
+        <v>9</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="5">
+        <v>10</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="5">
+        <v>11</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="30">
+      <c r="A41" s="5">
+        <v>12</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E41" s="7">
+        <v>149</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="4" t="s">
+    <row r="45" spans="1:6">
+      <c r="A45" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7" t="s">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="5"/>
+      <c r="B46" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C46" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D46" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E46" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="7">
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" ht="35.25" customHeight="1">
+      <c r="A47" s="5">
         <v>1</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="7">
+      <c r="B47" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" ht="30">
+      <c r="A48" s="5">
         <v>2</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="7">
+      <c r="B48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" ht="29.25" customHeight="1">
+      <c r="A49" s="5">
         <v>3</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:6" ht="30">
-      <c r="A36" s="7">
+      <c r="B49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5">
         <v>4</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="7">
+      <c r="B50" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" ht="30">
+      <c r="A51" s="5">
         <v>5</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6" ht="30">
-      <c r="A38" s="7">
+      <c r="B51" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" ht="30">
+      <c r="A52" s="5">
         <v>6</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:6" ht="30">
-      <c r="A39" s="7">
+      <c r="B52" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="5">
         <v>7</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:6" ht="60">
-      <c r="A40" s="7">
+      <c r="B53" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="5">
         <v>8</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="E40" s="7">
-        <v>158</v>
-      </c>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:6" ht="30">
-      <c r="A41" s="7">
+      <c r="B54" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="5">
         <v>9</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="7">
+      <c r="B55" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="5">
         <v>10</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="7">
+      <c r="B56" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" ht="30">
+      <c r="A57" s="5">
         <v>11</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:6" ht="30">
-      <c r="A44" s="7">
-        <v>12</v>
-      </c>
-      <c r="B44" s="7" t="s">
+      <c r="B57" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E44" s="7">
-        <v>149</v>
-      </c>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="7">
-        <v>1</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" ht="30">
-      <c r="A50" s="7">
-        <v>2</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="7">
-        <v>3</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="7">
-        <v>4</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="1:6" ht="30">
-      <c r="A53" s="7">
-        <v>5</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-    </row>
-    <row r="54" spans="1:6" ht="30">
-      <c r="A54" s="7">
-        <v>6</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="7">
-        <v>7</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="7">
-        <v>8</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="7">
-        <v>9</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
+      <c r="C57" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="7">
-        <v>10</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2969,1309 +3126,2009 @@
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>246</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="30">
-      <c r="A63" s="7">
+      <c r="A63" s="5">
         <v>1</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
+      <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7" t="s">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D64" s="7"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" ht="30">
-      <c r="A65" s="7">
+      <c r="A65" s="5">
         <v>2</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="5" t="s">
         <v>220</v>
       </c>
       <c r="E65" s="7">
         <v>161</v>
       </c>
-      <c r="F65" s="7"/>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" ht="30">
-      <c r="A66" s="7">
+      <c r="A66" s="5">
         <v>3</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
+      <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
+      <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="7">
+      <c r="A68" s="5">
         <v>4</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="5" t="s">
         <v>223</v>
       </c>
       <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
+      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="30">
-      <c r="A69" s="7">
+      <c r="A69" s="5">
         <v>5</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
+      <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" ht="45">
-      <c r="A70" s="7">
+      <c r="A70" s="5">
         <v>6</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
+      <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
+      <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="7">
+      <c r="A72" s="5">
         <v>7</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7" t="s">
+      <c r="C72" s="5"/>
+      <c r="D72" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
+      <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" ht="45">
-      <c r="A73" s="7">
+      <c r="A73" s="5">
         <v>8</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="5" t="s">
         <v>224</v>
       </c>
       <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" ht="30">
-      <c r="A74" s="7">
+      <c r="A74" s="5">
         <v>9</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="5" t="s">
         <v>224</v>
       </c>
       <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="7">
+      <c r="A75" s="5">
         <v>10</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C75" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="5" t="s">
         <v>224</v>
       </c>
       <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
+      <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="7">
+      <c r="A76" s="5">
         <v>11</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
+      <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7" t="s">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D77" s="7"/>
+      <c r="D77" s="5"/>
       <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
+      <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="7">
+      <c r="A78" s="5">
         <v>12</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="5" t="s">
         <v>224</v>
       </c>
       <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
+      <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="7">
+      <c r="A79" s="5">
         <v>13</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="5" t="s">
         <v>224</v>
       </c>
       <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
+      <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="7">
+      <c r="A80" s="5">
         <v>14</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7" t="s">
+      <c r="C80" s="5"/>
+      <c r="D80" s="5" t="s">
         <v>224</v>
       </c>
       <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
+      <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" ht="30">
-      <c r="A81" s="7">
+      <c r="A81" s="5">
         <v>15</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
+      <c r="F81" s="5"/>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="7">
+      <c r="A82" s="5">
         <v>16</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="5" t="s">
         <v>222</v>
       </c>
       <c r="E82" s="7">
         <v>160</v>
       </c>
-      <c r="F82" s="7"/>
+      <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7" t="s">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C83" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="5" t="s">
         <v>227</v>
       </c>
       <c r="E83" s="7">
         <v>162</v>
       </c>
-      <c r="F83" s="7"/>
+      <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="B88" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" ht="45">
+      <c r="A89" s="5">
+        <v>1</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" ht="30">
+      <c r="A90" s="5">
+        <v>2</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="1:6" ht="45">
+      <c r="A91" s="5">
+        <v>3</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" ht="30">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E92" s="7">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="7"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="3" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" t="s">
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" s="4" t="s">
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7" t="s">
+      <c r="C96" s="1"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="5"/>
+      <c r="B97" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C97" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D97" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E87" s="7" t="s">
+      <c r="E97" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F87" s="7"/>
-    </row>
-    <row r="88" spans="1:6" ht="30">
-      <c r="A88" s="7">
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" ht="30">
+      <c r="A98" s="5">
         <v>1</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B98" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C98" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-    </row>
-    <row r="89" spans="1:6" ht="30">
-      <c r="A89" s="7">
+      <c r="D98" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E98" s="7"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" ht="30">
+      <c r="A99" s="5">
         <v>2</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B99" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C99" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D99" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-    </row>
-    <row r="90" spans="1:6" ht="30">
-      <c r="A90" s="7">
+      <c r="E99" s="7"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" ht="30">
+      <c r="A100" s="5">
         <v>3</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B100" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C100" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D100" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7"/>
-    </row>
-    <row r="91" spans="1:6" ht="30">
-      <c r="A91" s="7">
+      <c r="E100" s="7"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" ht="30">
+      <c r="A101" s="5">
         <v>4</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B101" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C101" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="7">
+      <c r="D101" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E101" s="7"/>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="5">
         <v>5</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B102" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C102" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-    </row>
-    <row r="93" spans="1:6" ht="30">
-      <c r="A93" s="7">
+      <c r="D102" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E102" s="7"/>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" ht="30">
+      <c r="A103" s="5">
         <v>6</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B103" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C103" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="D93" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="9">
+      <c r="D103" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E103" s="7"/>
+      <c r="F103" s="5"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="17">
         <v>7</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B104" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C104" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D94" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="7" t="s">
+      <c r="D104" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E104" s="7"/>
+      <c r="F104" s="5"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="17"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="7" t="s">
+      <c r="D105" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E105" s="7"/>
+      <c r="F105" s="5"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="17"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D96" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="9"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="7" t="s">
+      <c r="D106" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E106" s="7"/>
+      <c r="F106" s="5"/>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="17"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D97" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="7" t="s">
+      <c r="D107" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E107" s="7"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="17"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D98" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="9">
+      <c r="D108" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E108" s="7"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="17">
         <v>8</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B109" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="C109" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7">
+      <c r="D109" s="5"/>
+      <c r="E109" s="7">
         <v>177</v>
       </c>
-      <c r="F99" s="7"/>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="7" t="s">
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="17"/>
+      <c r="B110" s="17"/>
+      <c r="C110" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7">
+      <c r="D110" s="5"/>
+      <c r="E110" s="7">
         <v>178</v>
       </c>
-      <c r="F100" s="7"/>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="4" t="s">
+      <c r="F110" s="5"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="6"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="5"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="3" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" t="s">
+      <c r="E112" s="9"/>
+      <c r="F112" s="5"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="4" t="s">
+      <c r="E113" s="9"/>
+      <c r="F113" s="5"/>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C103" s="1"/>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7" t="s">
+      <c r="C114" s="1"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="5"/>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="8"/>
+      <c r="B115" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C115" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D115" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E104" s="7" t="s">
+      <c r="E115" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F104" s="7"/>
-    </row>
-    <row r="105" spans="1:6" ht="30">
-      <c r="A105" s="7">
+      <c r="F115" s="5"/>
+    </row>
+    <row r="116" spans="1:6" ht="30">
+      <c r="A116" s="5">
         <v>1</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B116" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C116" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E105" s="7"/>
-      <c r="F105" s="7"/>
-    </row>
-    <row r="106" spans="1:6" ht="30">
-      <c r="A106" s="7">
+      <c r="D116" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E116" s="7"/>
+      <c r="F116" s="5"/>
+    </row>
+    <row r="117" spans="1:6" ht="30">
+      <c r="A117" s="5">
         <v>2</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B117" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C117" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E106" s="7"/>
-      <c r="F106" s="7"/>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="7">
+      <c r="D117" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E117" s="7"/>
+      <c r="F117" s="5"/>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="5">
         <v>3</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B118" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C118" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="D118" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="E107" s="7">
+      <c r="E118" s="7">
         <v>152</v>
       </c>
-      <c r="F107" s="7"/>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="7">
+      <c r="F118" s="5"/>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="5">
         <v>4</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B119" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C119" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D108" s="7"/>
-      <c r="E108" s="7" t="s">
+      <c r="D119" s="5"/>
+      <c r="E119" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="F108" s="7"/>
-    </row>
-    <row r="109" spans="1:6" ht="30">
-      <c r="A109" s="7">
+      <c r="F119" s="5"/>
+    </row>
+    <row r="120" spans="1:6" ht="30">
+      <c r="A120" s="5">
         <v>5</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B120" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C120" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D109" s="7"/>
-      <c r="E109" s="7" t="s">
+      <c r="D120" s="5"/>
+      <c r="E120" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="F109" s="7"/>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="9">
+      <c r="F120" s="5"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="17">
         <v>6</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B121" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C121" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="D110" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E110" s="7"/>
-      <c r="F110" s="7"/>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="9"/>
-      <c r="B111" s="9"/>
-      <c r="C111" s="7" t="s">
+      <c r="D121" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E121" s="7"/>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="17"/>
+      <c r="B122" s="17"/>
+      <c r="C122" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D111" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112" s="9"/>
-      <c r="B112" s="9"/>
-      <c r="C112" s="7" t="s">
+      <c r="D122" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E122" s="7"/>
+      <c r="F122" s="5"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="17"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D112" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E112" s="7"/>
-      <c r="F112" s="7"/>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113" s="9"/>
-      <c r="B113" s="9"/>
-      <c r="C113" s="7" t="s">
+      <c r="D123" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E123" s="7"/>
+      <c r="F123" s="5"/>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="17"/>
+      <c r="B124" s="17"/>
+      <c r="C124" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="9"/>
-      <c r="B114" s="9"/>
-      <c r="C114" s="7" t="s">
+      <c r="D124" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E124" s="7"/>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="17"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D114" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
-    </row>
-    <row r="115" spans="1:6" ht="30">
-      <c r="A115" s="9">
+      <c r="D125" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E125" s="7"/>
+    </row>
+    <row r="126" spans="1:6" ht="30">
+      <c r="A126" s="17">
         <v>7</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="B126" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C126" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="D115" s="7" t="s">
+      <c r="D126" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="E115" s="7">
+      <c r="E126" s="7">
         <v>142</v>
       </c>
-      <c r="F115" s="7"/>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116" s="9"/>
-      <c r="B116" s="9"/>
-      <c r="C116" s="7" t="s">
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="17"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D116" s="7" t="s">
+      <c r="D127" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="E116" s="7">
+      <c r="E127" s="7">
         <v>139</v>
       </c>
-      <c r="F116" s="7"/>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" s="4" t="s">
+      <c r="F127" s="5"/>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="6"/>
+      <c r="B128" s="6"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="5"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="3" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" t="s">
+      <c r="F129" s="5"/>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119" s="4" t="s">
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" ht="30">
-      <c r="A120" s="7">
+      <c r="C131" s="1"/>
+      <c r="F131" s="5"/>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="8"/>
+      <c r="B132" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E132" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" ht="30">
+      <c r="A133" s="5">
         <v>1</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="B133" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C133" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="D120" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" s="7">
+      <c r="D133" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="5">
         <v>2</v>
       </c>
-      <c r="B121" s="7" t="s">
+      <c r="B134" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C134" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="D121" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E121" s="7"/>
-      <c r="F121" s="7"/>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" s="9">
+      <c r="D134" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="17">
         <v>3</v>
       </c>
-      <c r="B122" s="9" t="s">
+      <c r="B135" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="C135" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" s="9"/>
-      <c r="B123" s="9"/>
-      <c r="C123" s="7" t="s">
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="17"/>
+      <c r="B136" s="17"/>
+      <c r="C136" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D123" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="9"/>
-      <c r="B124" s="9"/>
-      <c r="C124" s="7" t="s">
+      <c r="D136" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="17"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D124" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E124" s="7"/>
-      <c r="F124" s="7"/>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="9"/>
-      <c r="B125" s="9"/>
-      <c r="C125" s="7" t="s">
+      <c r="D137" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="17"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D125" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E125" s="7"/>
-      <c r="F125" s="7"/>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="9"/>
-      <c r="B126" s="9"/>
-      <c r="C126" s="7" t="s">
+      <c r="D138" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="17"/>
+      <c r="B139" s="17"/>
+      <c r="C139" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D126" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E126" s="7"/>
-      <c r="F126" s="7"/>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="9"/>
-      <c r="B127" s="9"/>
-      <c r="C127" s="7" t="s">
+      <c r="D139" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="17"/>
+      <c r="B140" s="17"/>
+      <c r="C140" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D127" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" s="9"/>
-      <c r="B128" s="9"/>
-      <c r="C128" s="7" t="s">
+      <c r="D140" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="17"/>
+      <c r="B141" s="17"/>
+      <c r="C141" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D128" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E128" s="7"/>
-      <c r="F128" s="7"/>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" s="9"/>
-      <c r="B129" s="9"/>
-      <c r="C129" s="7" t="s">
+      <c r="D141" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="17"/>
+      <c r="B142" s="17"/>
+      <c r="C142" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D129" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E129" s="7"/>
-      <c r="F129" s="7"/>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" s="9"/>
-      <c r="B130" s="9"/>
-      <c r="C130" s="7" t="s">
+      <c r="D142" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="17"/>
+      <c r="B143" s="17"/>
+      <c r="C143" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D130" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E130" s="7"/>
-      <c r="F130" s="7"/>
-    </row>
-    <row r="131" spans="1:6">
-      <c r="A131" s="9"/>
-      <c r="B131" s="9"/>
-      <c r="C131" s="7" t="s">
+      <c r="D143" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="17"/>
+      <c r="B144" s="17"/>
+      <c r="C144" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D131" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E131" s="7"/>
-      <c r="F131" s="7"/>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" s="9"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="7" t="s">
+      <c r="D144" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="17"/>
+      <c r="B145" s="17"/>
+      <c r="C145" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D132" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" s="9"/>
-      <c r="B133" s="9"/>
-      <c r="C133" s="7" t="s">
+      <c r="D145" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="17"/>
+      <c r="B146" s="17"/>
+      <c r="C146" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D133" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E133" s="7"/>
-      <c r="F133" s="7"/>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" s="9"/>
-      <c r="B134" s="9"/>
-      <c r="C134" s="7" t="s">
+      <c r="D146" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="17"/>
+      <c r="B147" s="17"/>
+      <c r="C147" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D134" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E134" s="7"/>
-      <c r="F134" s="7"/>
-    </row>
-    <row r="135" spans="1:6">
-      <c r="A135" s="9"/>
-      <c r="B135" s="9"/>
-      <c r="C135" s="7" t="s">
+      <c r="D147" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="17"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D135" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E135" s="7"/>
-      <c r="F135" s="7"/>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="9"/>
-      <c r="B136" s="9"/>
-      <c r="C136" s="7" t="s">
+      <c r="D148" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5"/>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="17"/>
+      <c r="B149" s="17"/>
+      <c r="C149" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D136" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E136" s="7"/>
-      <c r="F136" s="7"/>
-    </row>
-    <row r="137" spans="1:6">
-      <c r="A137" s="9"/>
-      <c r="B137" s="9"/>
-      <c r="C137" s="7" t="s">
+      <c r="D149" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="17"/>
+      <c r="B150" s="17"/>
+      <c r="C150" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D137" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E137" s="7"/>
-      <c r="F137" s="7"/>
-    </row>
-    <row r="138" spans="1:6">
-      <c r="A138" s="9"/>
-      <c r="B138" s="9"/>
-      <c r="C138" s="7" t="s">
+      <c r="D150" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="17"/>
+      <c r="B151" s="17"/>
+      <c r="C151" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D138" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E138" s="7"/>
-      <c r="F138" s="7"/>
-    </row>
-    <row r="139" spans="1:6">
-      <c r="A139" s="9"/>
-      <c r="B139" s="9"/>
-      <c r="C139" s="7" t="s">
+      <c r="D151" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="17"/>
+      <c r="B152" s="17"/>
+      <c r="C152" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D139" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
-    </row>
-    <row r="140" spans="1:6">
-      <c r="A140" s="9"/>
-      <c r="B140" s="9"/>
-      <c r="C140" s="7" t="s">
+      <c r="D152" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="17"/>
+      <c r="B153" s="17"/>
+      <c r="C153" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="D140" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" s="9"/>
-      <c r="B141" s="9"/>
-      <c r="C141" s="7" t="s">
+      <c r="D153" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="17"/>
+      <c r="B154" s="17"/>
+      <c r="C154" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D141" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="A142" s="9"/>
-      <c r="B142" s="9"/>
-      <c r="C142" s="7" t="s">
+      <c r="D154" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="17"/>
+      <c r="B155" s="17"/>
+      <c r="C155" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D142" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7"/>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" s="9"/>
-      <c r="B143" s="9"/>
-      <c r="C143" s="7" t="s">
+      <c r="D155" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="17"/>
+      <c r="B156" s="17"/>
+      <c r="C156" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="D143" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E143" s="7"/>
-      <c r="F143" s="7"/>
-    </row>
-    <row r="144" spans="1:6">
-      <c r="A144" s="9"/>
-      <c r="B144" s="9"/>
-      <c r="C144" s="7" t="s">
+      <c r="D156" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="17"/>
+      <c r="B157" s="17"/>
+      <c r="C157" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D144" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E144" s="7"/>
-      <c r="F144" s="7"/>
-    </row>
-    <row r="145" spans="1:6">
-      <c r="A145" s="9"/>
-      <c r="B145" s="9"/>
-      <c r="C145" s="7" t="s">
+      <c r="D157" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="17"/>
+      <c r="B158" s="17"/>
+      <c r="C158" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D145" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E145" s="7"/>
-      <c r="F145" s="7"/>
-    </row>
-    <row r="146" spans="1:6">
-      <c r="A146" s="9"/>
-      <c r="B146" s="9"/>
-      <c r="C146" s="7" t="s">
+      <c r="D158" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E158" s="5"/>
+      <c r="F158" s="5"/>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="17"/>
+      <c r="B159" s="17"/>
+      <c r="C159" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D146" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E146" s="7"/>
-      <c r="F146" s="7"/>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" s="9">
+      <c r="D159" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="17">
         <v>4</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B160" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="C147" s="7" t="s">
+      <c r="C160" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" s="9"/>
-      <c r="B148" s="9"/>
-      <c r="C148" s="7" t="s">
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="17"/>
+      <c r="B161" s="17"/>
+      <c r="C161" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D148" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E148" s="7"/>
-      <c r="F148" s="7"/>
-    </row>
-    <row r="149" spans="1:6">
-      <c r="A149" s="9"/>
-      <c r="B149" s="9"/>
-      <c r="C149" s="7" t="s">
+      <c r="D161" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E161" s="5"/>
+      <c r="F161" s="5"/>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="17"/>
+      <c r="B162" s="17"/>
+      <c r="C162" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D149" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7"/>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="A150" s="9"/>
-      <c r="B150" s="9"/>
-      <c r="C150" s="7" t="s">
+      <c r="D162" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E162" s="5"/>
+      <c r="F162" s="5"/>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="17"/>
+      <c r="B163" s="17"/>
+      <c r="C163" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D150" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E150" s="7"/>
-      <c r="F150" s="7"/>
-    </row>
-    <row r="151" spans="1:6" ht="45">
-      <c r="A151" s="7">
+      <c r="D163" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E163" s="5"/>
+      <c r="F163" s="5"/>
+    </row>
+    <row r="164" spans="1:6" ht="45">
+      <c r="A164" s="5">
         <v>5</v>
       </c>
-      <c r="B151" s="7" t="s">
+      <c r="B164" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C151" s="7" t="s">
+      <c r="C164" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="D151" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E151" s="7"/>
-      <c r="F151" s="7"/>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="7"/>
-      <c r="D152" s="7"/>
-      <c r="E152" s="7"/>
-      <c r="F152" s="7"/>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="7"/>
-      <c r="D153" s="7"/>
-      <c r="E153" s="7"/>
-      <c r="F153" s="7"/>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154" s="7"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
-      <c r="C155" s="7"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
-      <c r="F155" s="7"/>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="A156" s="7"/>
-      <c r="B156" s="7"/>
-      <c r="C156" s="7"/>
-      <c r="D156" s="7"/>
-      <c r="E156" s="7"/>
-      <c r="F156" s="7"/>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="A157" s="7"/>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="7"/>
-      <c r="F157" s="7"/>
-    </row>
-    <row r="158" spans="1:6">
-      <c r="A158" s="7"/>
-      <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="7"/>
-      <c r="F158" s="7"/>
-    </row>
-    <row r="159" spans="1:6">
-      <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
-      <c r="C159" s="7"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
-    </row>
-    <row r="160" spans="1:6">
-      <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
-    </row>
-    <row r="161" spans="1:6">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="7"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="7"/>
-      <c r="F161" s="7"/>
-    </row>
-    <row r="162" spans="1:6">
-      <c r="A162" s="7"/>
-      <c r="B162" s="7"/>
-      <c r="C162" s="7"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="7"/>
-      <c r="F162" s="7"/>
-    </row>
-    <row r="163" spans="1:6">
-      <c r="A163" s="7"/>
-      <c r="B163" s="7"/>
-      <c r="C163" s="7"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="7"/>
-      <c r="F163" s="7"/>
-    </row>
-    <row r="164" spans="1:6">
-      <c r="A164" s="7"/>
-      <c r="B164" s="7"/>
-      <c r="C164" s="7"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="7"/>
-      <c r="F164" s="7"/>
+      <c r="D164" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E164" s="5"/>
+      <c r="F164" s="5"/>
     </row>
     <row r="165" spans="1:6">
-      <c r="A165" s="7"/>
-      <c r="B165" s="7"/>
-      <c r="C165" s="7"/>
-      <c r="D165" s="7"/>
-      <c r="E165" s="7"/>
-      <c r="F165" s="7"/>
+      <c r="A165" s="5"/>
+      <c r="B165" s="5"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="5"/>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F166" s="5"/>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" t="s">
+        <v>283</v>
+      </c>
+      <c r="F167" s="5"/>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C168" s="1"/>
+      <c r="F168" s="5"/>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="8"/>
+      <c r="B169" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D169" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E169" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F169" s="5"/>
+    </row>
+    <row r="170" spans="1:6" ht="30">
+      <c r="A170" s="10">
+        <v>1</v>
+      </c>
+      <c r="B170" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C170" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+    </row>
+    <row r="171" spans="1:6" ht="30">
+      <c r="A171" s="10">
+        <v>2</v>
+      </c>
+      <c r="B171" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C171" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+      <c r="F171" s="5"/>
+    </row>
+    <row r="172" spans="1:6" ht="30">
+      <c r="A172" s="10">
+        <v>3</v>
+      </c>
+      <c r="B172" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C172" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+    </row>
+    <row r="173" spans="1:6" ht="60">
+      <c r="A173" s="10">
+        <v>4</v>
+      </c>
+      <c r="B173" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C173" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+    </row>
+    <row r="174" spans="1:6" ht="54" customHeight="1">
+      <c r="A174" s="10">
+        <v>5</v>
+      </c>
+      <c r="B174" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C174" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="10">
+        <v>6</v>
+      </c>
+      <c r="B175" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C175" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="10">
+        <v>7</v>
+      </c>
+      <c r="B176" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C176" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="16">
+        <v>8</v>
+      </c>
+      <c r="B177" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="16"/>
+      <c r="B178" s="15"/>
+      <c r="C178" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="16"/>
+      <c r="B179" s="15"/>
+      <c r="C179" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="16"/>
+      <c r="B180" s="15"/>
+      <c r="C180" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="16"/>
+      <c r="B181" s="15"/>
+      <c r="C181" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="16"/>
+      <c r="B182" s="15"/>
+      <c r="C182" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="16"/>
+      <c r="B183" s="15"/>
+      <c r="C183" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="16"/>
+      <c r="B184" s="15"/>
+      <c r="C184" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="10">
+        <v>9</v>
+      </c>
+      <c r="B185" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="10">
+        <v>10</v>
+      </c>
+      <c r="B186" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C186" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="10"/>
+      <c r="B187" s="11"/>
+      <c r="C187" s="12"/>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C190" s="1"/>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="8"/>
+      <c r="B191" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D191" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="10">
+        <v>1</v>
+      </c>
+      <c r="B192" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C192" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D192" s="12"/>
+    </row>
+    <row r="193" spans="1:4" ht="30">
+      <c r="A193" s="10">
+        <v>2</v>
+      </c>
+      <c r="B193" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C193" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D193" s="12"/>
+    </row>
+    <row r="194" spans="1:4" ht="30">
+      <c r="A194" s="10">
+        <v>3</v>
+      </c>
+      <c r="B194" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C194" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D194" s="12"/>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="10">
+        <v>4</v>
+      </c>
+      <c r="B195" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C195" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D195" s="12"/>
+    </row>
+    <row r="196" spans="1:4" ht="30">
+      <c r="A196" s="10">
+        <v>5</v>
+      </c>
+      <c r="B196" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C196" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D196" s="12"/>
+    </row>
+    <row r="197" spans="1:4" ht="45">
+      <c r="A197" s="10">
+        <v>6</v>
+      </c>
+      <c r="B197" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C197" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D197" s="12"/>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="10">
+        <v>7</v>
+      </c>
+      <c r="B198" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C198" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D198" s="12"/>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="10">
+        <v>8</v>
+      </c>
+      <c r="B199" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C199" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D199" s="12"/>
+    </row>
+    <row r="200" spans="1:4" ht="30">
+      <c r="A200" s="10">
+        <v>9</v>
+      </c>
+      <c r="B200" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C200" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D200" s="12"/>
+    </row>
+    <row r="201" spans="1:4" ht="30">
+      <c r="A201" s="10">
+        <v>10</v>
+      </c>
+      <c r="B201" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C201" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D201" s="12"/>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="10">
+        <v>12</v>
+      </c>
+      <c r="B202" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C202" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D202" s="12"/>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="10">
+        <v>13</v>
+      </c>
+      <c r="B203" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C203" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D203" s="12"/>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="10">
+        <v>14</v>
+      </c>
+      <c r="B204" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C204" s="12"/>
+      <c r="D204" s="12"/>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="10"/>
+      <c r="B205" s="12"/>
+      <c r="C205" s="12"/>
+      <c r="D205" s="12"/>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C208" s="1"/>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="8"/>
+      <c r="B209" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D209" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210">
+        <v>1</v>
+      </c>
+      <c r="B210" t="s">
+        <v>100</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211">
+        <v>2</v>
+      </c>
+      <c r="B211" t="s">
+        <v>52</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212">
+        <v>3</v>
+      </c>
+      <c r="B212" t="s">
+        <v>104</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213">
+        <v>4</v>
+      </c>
+      <c r="B213" t="s">
+        <v>53</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214">
+        <v>5</v>
+      </c>
+      <c r="B214" t="s">
+        <v>107</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215">
+        <v>6</v>
+      </c>
+      <c r="B215" t="s">
+        <v>109</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216">
+        <v>7</v>
+      </c>
+      <c r="B216" t="s">
+        <v>111</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217">
+        <v>7</v>
+      </c>
+      <c r="B217" t="s">
+        <v>62</v>
+      </c>
+      <c r="C217" s="2"/>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="C218" s="2"/>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C221" s="1"/>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" s="8"/>
+      <c r="B222" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C222" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D222" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E222" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="30">
+      <c r="A223" s="14">
+        <v>1</v>
+      </c>
+      <c r="B223" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C223" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D223" s="12"/>
+      <c r="E223" s="13"/>
+    </row>
+    <row r="224" spans="1:5" ht="30">
+      <c r="A224" s="14">
+        <v>2</v>
+      </c>
+      <c r="B224" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C224" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D224" s="12"/>
+      <c r="E224" s="13"/>
+    </row>
+    <row r="225" spans="1:5" ht="30">
+      <c r="A225" s="14">
+        <v>3</v>
+      </c>
+      <c r="B225" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C225" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D225" s="12"/>
+      <c r="E225" s="13"/>
+    </row>
+    <row r="226" spans="1:5" ht="30">
+      <c r="A226" s="14">
+        <v>4</v>
+      </c>
+      <c r="B226" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C226" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D226" s="12"/>
+      <c r="E226" s="13"/>
+    </row>
+    <row r="227" spans="1:5" ht="30">
+      <c r="A227" s="14">
+        <v>5</v>
+      </c>
+      <c r="B227" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C227" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D227" s="12"/>
+      <c r="E227" s="13"/>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" s="14">
+        <v>6</v>
+      </c>
+      <c r="B228" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C228" s="12"/>
+      <c r="D228" s="12"/>
+      <c r="E228" s="13"/>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" s="14">
+        <v>7</v>
+      </c>
+      <c r="B229" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C229" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D229" s="12"/>
+      <c r="E229" s="13"/>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" s="14">
+        <v>8</v>
+      </c>
+      <c r="B230" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C230" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D230" s="12"/>
+      <c r="E230" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A110:A114"/>
-    <mergeCell ref="B110:B114"/>
-    <mergeCell ref="A147:A150"/>
-    <mergeCell ref="B147:B150"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="B122:B146"/>
-    <mergeCell ref="A122:A146"/>
-    <mergeCell ref="B15:B23"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="A99:A100"/>
+  <mergeCells count="16">
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="B121:B125"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="B104:B108"/>
+    <mergeCell ref="B177:B184"/>
+    <mergeCell ref="A177:A184"/>
+    <mergeCell ref="A160:A163"/>
+    <mergeCell ref="B160:B163"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B135:B159"/>
+    <mergeCell ref="A135:A159"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion del plan de testeo (hoja 3)
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="290">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -718,9 +718,6 @@
   </si>
   <si>
     <t>No debe de guardarse el usuario, el boton guardar debe estar desabilitado</t>
-  </si>
-  <si>
-    <t>xxx</t>
   </si>
   <si>
     <t>Permite ingresar el usuario sin seleccionar un rol.</t>
@@ -1163,16 +1160,16 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2378,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:IV26"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2401,33 +2398,33 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2475,7 +2472,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2487,10 +2484,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -2502,7 +2499,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>10</v>
@@ -2543,10 +2540,10 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -2558,8 +2555,8 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2569,8 +2566,8 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
@@ -2580,8 +2577,8 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
@@ -2591,8 +2588,8 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
@@ -2602,8 +2599,8 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
@@ -2613,8 +2610,8 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
@@ -2624,8 +2621,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="30">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
@@ -2675,33 +2672,33 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="5"/>
       <c r="B29" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F29" s="5"/>
     </row>
@@ -2807,7 +2804,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>218</v>
@@ -2823,10 +2820,10 @@
         <v>43</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="E37" s="7">
         <v>158</v>
@@ -2905,33 +2902,33 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="5"/>
       <c r="B46" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F46" s="5"/>
     </row>
@@ -3099,10 +3096,10 @@
         <v>217</v>
       </c>
       <c r="C57" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -3117,32 +3114,32 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:6">
       <c r="B62" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="30">
@@ -3197,7 +3194,7 @@
         <v>138</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>218</v>
@@ -3253,7 +3250,7 @@
         <v>143</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>218</v>
@@ -3288,7 +3285,7 @@
         <v>8</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>145</v>
@@ -3463,32 +3460,32 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:6">
       <c r="B88" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F88" s="5"/>
     </row>
@@ -3497,10 +3494,10 @@
         <v>1</v>
       </c>
       <c r="B89" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C89" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>218</v>
@@ -3513,10 +3510,10 @@
         <v>2</v>
       </c>
       <c r="B90" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C90" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>218</v>
@@ -3529,10 +3526,10 @@
         <v>3</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>218</v>
@@ -3546,10 +3543,10 @@
         <v>217</v>
       </c>
       <c r="C92" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>275</v>
       </c>
       <c r="E92" s="7">
         <v>179</v>
@@ -3564,19 +3561,19 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C96" s="1"/>
       <c r="F96" s="5"/>
@@ -3584,16 +3581,16 @@
     <row r="97" spans="1:6">
       <c r="A97" s="5"/>
       <c r="B97" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F97" s="5"/>
     </row>
@@ -3605,7 +3602,7 @@
         <v>160</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>218</v>
@@ -3653,7 +3650,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>218</v>
@@ -3685,7 +3682,7 @@
         <v>165</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>218</v>
@@ -3694,10 +3691,10 @@
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="17">
+      <c r="A104" s="16">
         <v>7</v>
       </c>
-      <c r="B104" s="17" t="s">
+      <c r="B104" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C104" s="5" t="s">
@@ -3710,8 +3707,8 @@
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="17"/>
-      <c r="B105" s="17"/>
+      <c r="A105" s="16"/>
+      <c r="B105" s="16"/>
       <c r="C105" s="5" t="s">
         <v>167</v>
       </c>
@@ -3722,8 +3719,8 @@
       <c r="F105" s="5"/>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
+      <c r="A106" s="16"/>
+      <c r="B106" s="16"/>
       <c r="C106" s="5" t="s">
         <v>168</v>
       </c>
@@ -3734,8 +3731,8 @@
       <c r="F106" s="5"/>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="17"/>
-      <c r="B107" s="17"/>
+      <c r="A107" s="16"/>
+      <c r="B107" s="16"/>
       <c r="C107" s="5" t="s">
         <v>169</v>
       </c>
@@ -3745,8 +3742,8 @@
       <c r="E107" s="7"/>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="17"/>
-      <c r="B108" s="17"/>
+      <c r="A108" s="16"/>
+      <c r="B108" s="16"/>
       <c r="C108" s="5" t="s">
         <v>170</v>
       </c>
@@ -3756,10 +3753,10 @@
       <c r="E108" s="7"/>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="17">
+      <c r="A109" s="16">
         <v>8</v>
       </c>
-      <c r="B109" s="17" t="s">
+      <c r="B109" s="16" t="s">
         <v>217</v>
       </c>
       <c r="C109" s="5" t="s">
@@ -3771,8 +3768,8 @@
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="17"/>
-      <c r="B110" s="17"/>
+      <c r="A110" s="16"/>
+      <c r="B110" s="16"/>
       <c r="C110" s="5" t="s">
         <v>232</v>
       </c>
@@ -3792,21 +3789,21 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E112" s="9"/>
       <c r="F112" s="5"/>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E113" s="9"/>
       <c r="F113" s="5"/>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C114" s="1"/>
       <c r="E114" s="9"/>
@@ -3815,16 +3812,16 @@
     <row r="115" spans="1:6">
       <c r="A115" s="8"/>
       <c r="B115" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F115" s="5"/>
     </row>
@@ -3836,7 +3833,7 @@
         <v>171</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>218</v>
@@ -3871,7 +3868,7 @@
         <v>174</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E118" s="7">
         <v>152</v>
@@ -3889,9 +3886,7 @@
         <v>176</v>
       </c>
       <c r="D119" s="5"/>
-      <c r="E119" s="7" t="s">
-        <v>234</v>
-      </c>
+      <c r="E119" s="7"/>
       <c r="F119" s="5"/>
     </row>
     <row r="120" spans="1:6" ht="30">
@@ -3902,19 +3897,17 @@
         <v>177</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D120" s="5"/>
-      <c r="E120" s="7" t="s">
-        <v>234</v>
-      </c>
+      <c r="E120" s="7"/>
       <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="17">
+      <c r="A121" s="16">
         <v>6</v>
       </c>
-      <c r="B121" s="17" t="s">
+      <c r="B121" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C121" s="5" t="s">
@@ -3927,8 +3920,8 @@
       <c r="F121" s="5"/>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
+      <c r="A122" s="16"/>
+      <c r="B122" s="16"/>
       <c r="C122" s="5" t="s">
         <v>179</v>
       </c>
@@ -3939,8 +3932,8 @@
       <c r="F122" s="5"/>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
+      <c r="A123" s="16"/>
+      <c r="B123" s="16"/>
       <c r="C123" s="5" t="s">
         <v>180</v>
       </c>
@@ -3951,8 +3944,8 @@
       <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="17"/>
-      <c r="B124" s="17"/>
+      <c r="A124" s="16"/>
+      <c r="B124" s="16"/>
       <c r="C124" s="5" t="s">
         <v>181</v>
       </c>
@@ -3962,8 +3955,8 @@
       <c r="E124" s="7"/>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="17"/>
-      <c r="B125" s="17"/>
+      <c r="A125" s="16"/>
+      <c r="B125" s="16"/>
       <c r="C125" s="5" t="s">
         <v>182</v>
       </c>
@@ -3973,30 +3966,30 @@
       <c r="E125" s="7"/>
     </row>
     <row r="126" spans="1:6" ht="30">
-      <c r="A126" s="17">
+      <c r="A126" s="16">
         <v>7</v>
       </c>
-      <c r="B126" s="17" t="s">
+      <c r="B126" s="16" t="s">
         <v>217</v>
       </c>
       <c r="C126" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D126" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="D126" s="5" t="s">
-        <v>237</v>
       </c>
       <c r="E126" s="7">
         <v>142</v>
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="17"/>
-      <c r="B127" s="17"/>
+      <c r="A127" s="16"/>
+      <c r="B127" s="16"/>
       <c r="C127" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D127" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="D127" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="E127" s="7">
         <v>139</v>
@@ -4013,19 +4006,19 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C131" s="1"/>
       <c r="F131" s="5"/>
@@ -4033,16 +4026,16 @@
     <row r="132" spans="1:6">
       <c r="A132" s="8"/>
       <c r="B132" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F132" s="5"/>
     </row>
@@ -4054,7 +4047,7 @@
         <v>183</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>218</v>
@@ -4079,10 +4072,10 @@
       <c r="F134" s="5"/>
     </row>
     <row r="135" spans="1:6">
-      <c r="A135" s="17">
+      <c r="A135" s="16">
         <v>3</v>
       </c>
-      <c r="B135" s="17" t="s">
+      <c r="B135" s="16" t="s">
         <v>184</v>
       </c>
       <c r="C135" s="5" t="s">
@@ -4093,8 +4086,8 @@
       <c r="F135" s="5"/>
     </row>
     <row r="136" spans="1:6">
-      <c r="A136" s="17"/>
-      <c r="B136" s="17"/>
+      <c r="A136" s="16"/>
+      <c r="B136" s="16"/>
       <c r="C136" s="5" t="s">
         <v>208</v>
       </c>
@@ -4105,8 +4098,8 @@
       <c r="F136" s="5"/>
     </row>
     <row r="137" spans="1:6">
-      <c r="A137" s="17"/>
-      <c r="B137" s="17"/>
+      <c r="A137" s="16"/>
+      <c r="B137" s="16"/>
       <c r="C137" s="5" t="s">
         <v>185</v>
       </c>
@@ -4117,8 +4110,8 @@
       <c r="F137" s="5"/>
     </row>
     <row r="138" spans="1:6">
-      <c r="A138" s="17"/>
-      <c r="B138" s="17"/>
+      <c r="A138" s="16"/>
+      <c r="B138" s="16"/>
       <c r="C138" s="5" t="s">
         <v>186</v>
       </c>
@@ -4129,8 +4122,8 @@
       <c r="F138" s="5"/>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" s="17"/>
-      <c r="B139" s="17"/>
+      <c r="A139" s="16"/>
+      <c r="B139" s="16"/>
       <c r="C139" s="5" t="s">
         <v>187</v>
       </c>
@@ -4141,8 +4134,8 @@
       <c r="F139" s="5"/>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="17"/>
-      <c r="B140" s="17"/>
+      <c r="A140" s="16"/>
+      <c r="B140" s="16"/>
       <c r="C140" s="5" t="s">
         <v>188</v>
       </c>
@@ -4153,8 +4146,8 @@
       <c r="F140" s="5"/>
     </row>
     <row r="141" spans="1:6">
-      <c r="A141" s="17"/>
-      <c r="B141" s="17"/>
+      <c r="A141" s="16"/>
+      <c r="B141" s="16"/>
       <c r="C141" s="5" t="s">
         <v>189</v>
       </c>
@@ -4165,8 +4158,8 @@
       <c r="F141" s="5"/>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="17"/>
-      <c r="B142" s="17"/>
+      <c r="A142" s="16"/>
+      <c r="B142" s="16"/>
       <c r="C142" s="5" t="s">
         <v>190</v>
       </c>
@@ -4177,8 +4170,8 @@
       <c r="F142" s="5"/>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="17"/>
-      <c r="B143" s="17"/>
+      <c r="A143" s="16"/>
+      <c r="B143" s="16"/>
       <c r="C143" s="5" t="s">
         <v>191</v>
       </c>
@@ -4189,8 +4182,8 @@
       <c r="F143" s="5"/>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="17"/>
-      <c r="B144" s="17"/>
+      <c r="A144" s="16"/>
+      <c r="B144" s="16"/>
       <c r="C144" s="5" t="s">
         <v>192</v>
       </c>
@@ -4201,8 +4194,8 @@
       <c r="F144" s="5"/>
     </row>
     <row r="145" spans="1:6">
-      <c r="A145" s="17"/>
-      <c r="B145" s="17"/>
+      <c r="A145" s="16"/>
+      <c r="B145" s="16"/>
       <c r="C145" s="5" t="s">
         <v>193</v>
       </c>
@@ -4213,8 +4206,8 @@
       <c r="F145" s="5"/>
     </row>
     <row r="146" spans="1:6">
-      <c r="A146" s="17"/>
-      <c r="B146" s="17"/>
+      <c r="A146" s="16"/>
+      <c r="B146" s="16"/>
       <c r="C146" s="5" t="s">
         <v>194</v>
       </c>
@@ -4225,8 +4218,8 @@
       <c r="F146" s="5"/>
     </row>
     <row r="147" spans="1:6">
-      <c r="A147" s="17"/>
-      <c r="B147" s="17"/>
+      <c r="A147" s="16"/>
+      <c r="B147" s="16"/>
       <c r="C147" s="5" t="s">
         <v>195</v>
       </c>
@@ -4237,8 +4230,8 @@
       <c r="F147" s="5"/>
     </row>
     <row r="148" spans="1:6">
-      <c r="A148" s="17"/>
-      <c r="B148" s="17"/>
+      <c r="A148" s="16"/>
+      <c r="B148" s="16"/>
       <c r="C148" s="5" t="s">
         <v>196</v>
       </c>
@@ -4249,8 +4242,8 @@
       <c r="F148" s="5"/>
     </row>
     <row r="149" spans="1:6">
-      <c r="A149" s="17"/>
-      <c r="B149" s="17"/>
+      <c r="A149" s="16"/>
+      <c r="B149" s="16"/>
       <c r="C149" s="5" t="s">
         <v>197</v>
       </c>
@@ -4261,8 +4254,8 @@
       <c r="F149" s="5"/>
     </row>
     <row r="150" spans="1:6">
-      <c r="A150" s="17"/>
-      <c r="B150" s="17"/>
+      <c r="A150" s="16"/>
+      <c r="B150" s="16"/>
       <c r="C150" s="5" t="s">
         <v>198</v>
       </c>
@@ -4273,8 +4266,8 @@
       <c r="F150" s="5"/>
     </row>
     <row r="151" spans="1:6">
-      <c r="A151" s="17"/>
-      <c r="B151" s="17"/>
+      <c r="A151" s="16"/>
+      <c r="B151" s="16"/>
       <c r="C151" s="5" t="s">
         <v>199</v>
       </c>
@@ -4285,8 +4278,8 @@
       <c r="F151" s="5"/>
     </row>
     <row r="152" spans="1:6">
-      <c r="A152" s="17"/>
-      <c r="B152" s="17"/>
+      <c r="A152" s="16"/>
+      <c r="B152" s="16"/>
       <c r="C152" s="5" t="s">
         <v>200</v>
       </c>
@@ -4297,8 +4290,8 @@
       <c r="F152" s="5"/>
     </row>
     <row r="153" spans="1:6">
-      <c r="A153" s="17"/>
-      <c r="B153" s="17"/>
+      <c r="A153" s="16"/>
+      <c r="B153" s="16"/>
       <c r="C153" s="5" t="s">
         <v>201</v>
       </c>
@@ -4309,8 +4302,8 @@
       <c r="F153" s="5"/>
     </row>
     <row r="154" spans="1:6">
-      <c r="A154" s="17"/>
-      <c r="B154" s="17"/>
+      <c r="A154" s="16"/>
+      <c r="B154" s="16"/>
       <c r="C154" s="5" t="s">
         <v>202</v>
       </c>
@@ -4321,8 +4314,8 @@
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6">
-      <c r="A155" s="17"/>
-      <c r="B155" s="17"/>
+      <c r="A155" s="16"/>
+      <c r="B155" s="16"/>
       <c r="C155" s="5" t="s">
         <v>203</v>
       </c>
@@ -4333,8 +4326,8 @@
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6">
-      <c r="A156" s="17"/>
-      <c r="B156" s="17"/>
+      <c r="A156" s="16"/>
+      <c r="B156" s="16"/>
       <c r="C156" s="5" t="s">
         <v>204</v>
       </c>
@@ -4345,8 +4338,8 @@
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6">
-      <c r="A157" s="17"/>
-      <c r="B157" s="17"/>
+      <c r="A157" s="16"/>
+      <c r="B157" s="16"/>
       <c r="C157" s="5" t="s">
         <v>205</v>
       </c>
@@ -4357,8 +4350,8 @@
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6">
-      <c r="A158" s="17"/>
-      <c r="B158" s="17"/>
+      <c r="A158" s="16"/>
+      <c r="B158" s="16"/>
       <c r="C158" s="5" t="s">
         <v>206</v>
       </c>
@@ -4369,8 +4362,8 @@
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6">
-      <c r="A159" s="17"/>
-      <c r="B159" s="17"/>
+      <c r="A159" s="16"/>
+      <c r="B159" s="16"/>
       <c r="C159" s="5" t="s">
         <v>207</v>
       </c>
@@ -4381,10 +4374,10 @@
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6">
-      <c r="A160" s="17">
+      <c r="A160" s="16">
         <v>4</v>
       </c>
-      <c r="B160" s="17" t="s">
+      <c r="B160" s="16" t="s">
         <v>209</v>
       </c>
       <c r="C160" s="5" t="s">
@@ -4395,8 +4388,8 @@
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6">
-      <c r="A161" s="17"/>
-      <c r="B161" s="17"/>
+      <c r="A161" s="16"/>
+      <c r="B161" s="16"/>
       <c r="C161" s="5" t="s">
         <v>210</v>
       </c>
@@ -4407,8 +4400,8 @@
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6">
-      <c r="A162" s="17"/>
-      <c r="B162" s="17"/>
+      <c r="A162" s="16"/>
+      <c r="B162" s="16"/>
       <c r="C162" s="5" t="s">
         <v>211</v>
       </c>
@@ -4419,8 +4412,8 @@
       <c r="F162" s="5"/>
     </row>
     <row r="163" spans="1:6">
-      <c r="A163" s="17"/>
-      <c r="B163" s="17"/>
+      <c r="A163" s="16"/>
+      <c r="B163" s="16"/>
       <c r="C163" s="5" t="s">
         <v>212</v>
       </c>
@@ -4438,7 +4431,7 @@
         <v>216</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>218</v>
@@ -4456,19 +4449,19 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F166" s="5"/>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F167" s="5"/>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C168" s="1"/>
       <c r="F168" s="5"/>
@@ -4476,16 +4469,16 @@
     <row r="169" spans="1:6">
       <c r="A169" s="8"/>
       <c r="B169" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C169" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F169" s="5"/>
     </row>
@@ -4549,7 +4542,7 @@
         <v>5</v>
       </c>
       <c r="B174" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C174" s="12" t="s">
         <v>74</v>
@@ -4578,10 +4571,10 @@
       </c>
     </row>
     <row r="177" spans="1:5">
-      <c r="A177" s="16">
+      <c r="A177" s="18">
         <v>8</v>
       </c>
-      <c r="B177" s="15" t="s">
+      <c r="B177" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C177" s="12" t="s">
@@ -4589,50 +4582,50 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="16"/>
-      <c r="B178" s="15"/>
+      <c r="A178" s="18"/>
+      <c r="B178" s="17"/>
       <c r="C178" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:5">
-      <c r="A179" s="16"/>
-      <c r="B179" s="15"/>
+      <c r="A179" s="18"/>
+      <c r="B179" s="17"/>
       <c r="C179" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="180" spans="1:5">
-      <c r="A180" s="16"/>
-      <c r="B180" s="15"/>
+      <c r="A180" s="18"/>
+      <c r="B180" s="17"/>
       <c r="C180" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="181" spans="1:5">
-      <c r="A181" s="16"/>
-      <c r="B181" s="15"/>
+      <c r="A181" s="18"/>
+      <c r="B181" s="17"/>
       <c r="C181" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="182" spans="1:5">
-      <c r="A182" s="16"/>
-      <c r="B182" s="15"/>
+      <c r="A182" s="18"/>
+      <c r="B182" s="17"/>
       <c r="C182" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="16"/>
-      <c r="B183" s="15"/>
+      <c r="A183" s="18"/>
+      <c r="B183" s="17"/>
       <c r="C183" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="184" spans="1:5">
-      <c r="A184" s="16"/>
-      <c r="B184" s="15"/>
+      <c r="A184" s="18"/>
+      <c r="B184" s="17"/>
       <c r="C184" s="12" t="s">
         <v>80</v>
       </c>
@@ -4666,33 +4659,33 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C190" s="1"/>
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="8"/>
       <c r="B191" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C191" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E191" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4760,10 +4753,10 @@
         <v>6</v>
       </c>
       <c r="B197" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C197" s="12" t="s">
         <v>286</v>
-      </c>
-      <c r="C197" s="12" t="s">
-        <v>287</v>
       </c>
       <c r="D197" s="12"/>
     </row>
@@ -4799,7 +4792,7 @@
         <v>97</v>
       </c>
       <c r="C200" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D200" s="12"/>
     </row>
@@ -4811,7 +4804,7 @@
         <v>43</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D201" s="12"/>
     </row>
@@ -4857,33 +4850,33 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C208" s="1"/>
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="8"/>
       <c r="B209" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C209" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E209" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -4977,33 +4970,33 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C221" s="1"/>
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="8"/>
       <c r="B222" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C222" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D222" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E222" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="30">
@@ -5110,22 +5103,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="B177:B184"/>
+    <mergeCell ref="A177:A184"/>
+    <mergeCell ref="A160:A163"/>
+    <mergeCell ref="B160:B163"/>
     <mergeCell ref="A121:A125"/>
     <mergeCell ref="B121:B125"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B135:B159"/>
+    <mergeCell ref="A135:A159"/>
     <mergeCell ref="B15:B22"/>
     <mergeCell ref="A15:A22"/>
     <mergeCell ref="A104:A108"/>
     <mergeCell ref="B104:B108"/>
-    <mergeCell ref="B177:B184"/>
-    <mergeCell ref="A177:A184"/>
-    <mergeCell ref="A160:A163"/>
-    <mergeCell ref="B160:B163"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B135:B159"/>
-    <mergeCell ref="A135:A159"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="A109:A110"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizacion plan de testeo
</commit_message>
<xml_diff>
--- a/Testeo/Plan de Testo.xlsx
+++ b/Testeo/Plan de Testo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="289">
   <si>
     <t>Plan de Pruebas del Softaware</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Registrar un cliente, ingresar los campos obligatorios y guardar el cliente</t>
-  </si>
-  <si>
-    <t>Aparece un mensaje de confirmacion que el cliente se guardo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y aparece en la lista de clientes </t>
   </si>
   <si>
     <t>Registrar un cliente, sin ingresar todos los campos obligariorios</t>
@@ -1066,6 +1060,9 @@
       </rPr>
       <t>Buscar guía de transporte</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparece un mensaje de confirmacion que el cliente se guardoy aparece en la lista de clientes </t>
   </si>
 </sst>
 </file>
@@ -1160,9 +1157,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1170,6 +1164,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1504,12 +1501,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1523,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -1534,10 +1531,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1545,10 +1542,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1559,10 +1556,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1573,10 +1570,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1593,15 +1590,15 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="B18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -1613,10 +1610,10 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1627,10 +1624,10 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1641,45 +1638,45 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="C25" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="C26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="C27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="C28" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="C29" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="C30" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1690,10 +1687,10 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1701,10 +1698,10 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1718,7 +1715,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" s="2"/>
     </row>
@@ -1730,10 +1727,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1741,10 +1738,10 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1752,10 +1749,10 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1763,10 +1760,10 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1774,10 +1771,10 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1785,10 +1782,10 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1796,15 +1793,15 @@
     </row>
     <row r="46" spans="1:3">
       <c r="B46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="C47" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1812,10 +1809,10 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1823,10 +1820,10 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1834,15 +1831,15 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="C51" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1850,15 +1847,15 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="C53" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1869,10 +1866,10 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1880,10 +1877,10 @@
         <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1894,7 +1891,7 @@
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C58" s="2"/>
     </row>
@@ -1906,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C60" s="2"/>
     </row>
@@ -1915,10 +1912,10 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1926,10 +1923,10 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1937,10 +1934,10 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1948,10 +1945,10 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1959,10 +1956,10 @@
         <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1970,10 +1967,10 @@
         <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1981,10 +1978,10 @@
         <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1992,7 +1989,7 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C68" s="2"/>
     </row>
@@ -2004,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C70" s="2"/>
     </row>
@@ -2013,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2024,10 +2021,10 @@
         <v>2</v>
       </c>
       <c r="B72" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="30.75" customHeight="1">
@@ -2035,10 +2032,10 @@
         <v>3</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2046,10 +2043,10 @@
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="30.75" customHeight="1">
@@ -2057,10 +2054,10 @@
         <v>5</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2068,7 +2065,7 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C76" s="2"/>
     </row>
@@ -2077,10 +2074,10 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2088,10 +2085,10 @@
         <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2373,10 +2370,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G230"/>
+  <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2398,33 +2395,33 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2437,536 +2434,580 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>288</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>252</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+    <row r="9" spans="1:7" ht="60">
+      <c r="A9" s="5">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="45">
       <c r="A10" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>255</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="60">
+    <row r="11" spans="1:7">
       <c r="A11" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>255</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="45">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>257</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="5">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
+      <c r="A13" s="15">
+        <v>7</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E13" s="5"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="30">
-      <c r="A14" s="5">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
+    <row r="14" spans="1:7">
+      <c r="A14" s="15"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="16">
-        <v>7</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>15</v>
-      </c>
+      <c r="A15" s="15"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="16"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="16"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E19" s="5"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="16"/>
-      <c r="B20" s="15"/>
+    <row r="20" spans="1:7" ht="30">
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="16"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="5">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="30">
-      <c r="A22" s="16"/>
-      <c r="B22" s="15"/>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="5">
-        <v>8</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="5">
-        <v>9</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="A24" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="A25" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>246</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>243</v>
-      </c>
+      <c r="A27" s="5"/>
+      <c r="B27" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C28" s="1"/>
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="5"/>
-      <c r="B29" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>239</v>
-      </c>
+      <c r="A29" s="5">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="7"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="30">
       <c r="A31" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>218</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="7"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="30">
       <c r="A33" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="5"/>
+        <v>256</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E34" s="7"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="60">
       <c r="A35" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>40</v>
+        <v>257</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E35" s="7"/>
+        <v>258</v>
+      </c>
+      <c r="E35" s="7">
+        <v>158</v>
+      </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="30">
       <c r="A36" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>258</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="60">
+    <row r="37" spans="1:6">
       <c r="A37" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>259</v>
+        <v>46</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="E37" s="7">
-        <v>158</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="E37" s="7"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:6">
       <c r="A38" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D38" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="C39" s="5"/>
       <c r="D39" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E39" s="7"/>
+        <v>217</v>
+      </c>
+      <c r="E39" s="7">
+        <v>149</v>
+      </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="5">
-        <v>11</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>218</v>
-      </c>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="7"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" ht="30">
-      <c r="A41" s="5">
-        <v>12</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E41" s="7">
-        <v>149</v>
-      </c>
-      <c r="F41" s="5"/>
+    <row r="41" spans="1:6">
+      <c r="A41" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="5"/>
+      <c r="A42" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
-        <v>247</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="5"/>
-      <c r="B46" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="A44" s="5"/>
+      <c r="B44" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E46" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>239</v>
       </c>
+      <c r="E44" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" ht="35.25" customHeight="1">
+      <c r="A45" s="5">
+        <v>1</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" ht="30">
+      <c r="A46" s="5">
+        <v>2</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" ht="35.25" customHeight="1">
+    <row r="47" spans="1:6" ht="29.25" customHeight="1">
       <c r="A47" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" ht="30">
+    <row r="48" spans="1:6">
       <c r="A48" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D48" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" ht="29.25" customHeight="1">
+    <row r="49" spans="1:6" ht="30">
       <c r="A49" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>58</v>
@@ -2975,1532 +3016,1528 @@
         <v>59</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" ht="30">
       <c r="A50" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>218</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" ht="30">
+    <row r="51" spans="1:6">
       <c r="A51" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" ht="30">
+    <row r="52" spans="1:6">
       <c r="A52" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" ht="30">
       <c r="A55" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>129</v>
+        <v>215</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>130</v>
+        <v>269</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>218</v>
+        <v>270</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="5">
-        <v>10</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>218</v>
-      </c>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="5">
-        <v>11</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+    <row r="57" spans="1:6">
+      <c r="A57" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
+      <c r="A58" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="3" t="s">
-        <v>248</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C61" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="30">
+      <c r="A61" s="5">
+        <v>1</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E61" s="7"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="B62" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:6" ht="30">
       <c r="A63" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E63" s="7"/>
+      <c r="E63" s="7">
+        <v>161</v>
+      </c>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+    <row r="64" spans="1:6" ht="30">
+      <c r="A64" s="5">
+        <v>3</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="C64" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D64" s="5"/>
+        <v>259</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E64" s="7"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" ht="30">
-      <c r="A65" s="5">
-        <v>2</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C65" s="5" t="s">
+    <row r="65" spans="1:6">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="5">
+        <v>4</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E65" s="7">
-        <v>161</v>
-      </c>
-      <c r="F65" s="5"/>
-    </row>
-    <row r="66" spans="1:6" ht="30">
-      <c r="A66" s="5">
-        <v>3</v>
-      </c>
-      <c r="B66" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>261</v>
-      </c>
       <c r="D66" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+    <row r="67" spans="1:6" ht="30">
+      <c r="A67" s="5">
+        <v>5</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E67" s="7"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" ht="45">
       <c r="A68" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>140</v>
+        <v>260</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E68" s="7"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" ht="30">
-      <c r="A69" s="5">
-        <v>5</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>218</v>
-      </c>
+    <row r="69" spans="1:6">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="7"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" ht="45">
+    <row r="70" spans="1:6">
       <c r="A70" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>262</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C70" s="5"/>
       <c r="D70" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E70" s="7"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+    <row r="71" spans="1:6" ht="45">
+      <c r="A71" s="5">
+        <v>8</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="E71" s="7"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" ht="30">
       <c r="A72" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B72" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C72" s="5"/>
       <c r="D72" s="5" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E72" s="7"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" ht="45">
+    <row r="73" spans="1:6">
       <c r="A73" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>263</v>
+        <v>146</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" ht="30">
+    <row r="74" spans="1:6">
       <c r="A74" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E74" s="7"/>
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="5">
-        <v>10</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>148</v>
-      </c>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>224</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D75" s="5"/>
       <c r="E75" s="7"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E76" s="7"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="5">
+        <v>13</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="C77" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D77" s="5"/>
+        <v>154</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="E77" s="7"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="C78" s="5"/>
       <c r="D78" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E78" s="7"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" ht="30">
       <c r="A79" s="5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E79" s="7"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C80" s="5"/>
+        <v>215</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>219</v>
+      </c>
       <c r="D80" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E80" s="7">
+        <v>160</v>
+      </c>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E80" s="7"/>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81" spans="1:6" ht="30">
-      <c r="A81" s="5">
-        <v>15</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="C81" s="5" t="s">
-        <v>159</v>
+        <v>223</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E81" s="7"/>
+        <v>225</v>
+      </c>
+      <c r="E81" s="7">
+        <v>162</v>
+      </c>
       <c r="F81" s="5"/>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="5">
-        <v>16</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E82" s="7">
-        <v>160</v>
-      </c>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="7"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E83" s="7">
-        <v>162</v>
-      </c>
-      <c r="F83" s="5"/>
+      <c r="A83" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="5"/>
+      <c r="A84" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="3" t="s">
-        <v>248</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="B88" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C88" s="1" t="s">
+      <c r="B86" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E88" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="E86" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" spans="1:6" ht="45">
+      <c r="A87" s="5">
+        <v>1</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" ht="30">
+      <c r="A88" s="5">
+        <v>2</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E88" s="5"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" ht="45">
       <c r="A89" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B89" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C89" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C89" s="5" t="s">
-        <v>276</v>
-      </c>
       <c r="D89" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" ht="30">
-      <c r="A90" s="5">
-        <v>2</v>
-      </c>
+      <c r="A90" s="5"/>
       <c r="B90" s="5" t="s">
-        <v>279</v>
+        <v>215</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-    </row>
-    <row r="91" spans="1:6" ht="45">
-      <c r="A91" s="5">
-        <v>3</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" spans="1:6" ht="30">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E92" s="7">
+        <v>272</v>
+      </c>
+      <c r="E90" s="7">
         <v>179</v>
       </c>
     </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="7"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F92" s="5"/>
+    </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="7"/>
+      <c r="A93" t="s">
+        <v>248</v>
+      </c>
+      <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="3" t="s">
         <v>249</v>
       </c>
+      <c r="C94" s="1"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" t="s">
-        <v>250</v>
+      <c r="A95" s="5"/>
+      <c r="B95" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>237</v>
       </c>
       <c r="F95" s="5"/>
     </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C96" s="1"/>
+    <row r="96" spans="1:6" ht="30">
+      <c r="A96" s="5">
+        <v>1</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E96" s="7"/>
       <c r="F96" s="5"/>
     </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="5"/>
-      <c r="B97" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>239</v>
-      </c>
+    <row r="97" spans="1:6" ht="30">
+      <c r="A97" s="5">
+        <v>2</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E97" s="7"/>
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" ht="30">
       <c r="A98" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" ht="30">
       <c r="A99" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>228</v>
+        <v>160</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>229</v>
+        <v>263</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E99" s="7"/>
       <c r="F99" s="5"/>
     </row>
-    <row r="100" spans="1:6" ht="30">
+    <row r="100" spans="1:6">
       <c r="A100" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C100" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>230</v>
-      </c>
       <c r="D100" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" ht="30">
       <c r="A101" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E101" s="7"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="5">
-        <v>5</v>
-      </c>
-      <c r="B102" s="5" t="s">
+      <c r="A102" s="15">
+        <v>7</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C102" s="5" t="s">
-        <v>163</v>
-      </c>
       <c r="D102" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E102" s="7"/>
       <c r="F102" s="5"/>
     </row>
-    <row r="103" spans="1:6" ht="30">
-      <c r="A103" s="5">
-        <v>6</v>
-      </c>
-      <c r="B103" s="5" t="s">
+    <row r="103" spans="1:6">
+      <c r="A103" s="15"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C103" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="D103" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E103" s="7"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="16">
-        <v>7</v>
-      </c>
-      <c r="B104" s="16" t="s">
-        <v>15</v>
-      </c>
+      <c r="A104" s="15"/>
+      <c r="B104" s="15"/>
       <c r="C104" s="5" t="s">
         <v>166</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E104" s="7"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="16"/>
-      <c r="B105" s="16"/>
+      <c r="A105" s="15"/>
+      <c r="B105" s="15"/>
       <c r="C105" s="5" t="s">
         <v>167</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E105" s="7"/>
-      <c r="F105" s="5"/>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="16"/>
-      <c r="B106" s="16"/>
+      <c r="A106" s="15"/>
+      <c r="B106" s="15"/>
       <c r="C106" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E106" s="7"/>
-      <c r="F106" s="5"/>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="16"/>
-      <c r="B107" s="16"/>
+      <c r="A107" s="15">
+        <v>8</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>215</v>
+      </c>
       <c r="C107" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E107" s="7"/>
+        <v>229</v>
+      </c>
+      <c r="D107" s="5"/>
+      <c r="E107" s="7">
+        <v>177</v>
+      </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="16"/>
-      <c r="B108" s="16"/>
+      <c r="A108" s="15"/>
+      <c r="B108" s="15"/>
       <c r="C108" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E108" s="7"/>
+        <v>230</v>
+      </c>
+      <c r="D108" s="5"/>
+      <c r="E108" s="7">
+        <v>178</v>
+      </c>
+      <c r="F108" s="5"/>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="16">
-        <v>8</v>
-      </c>
-      <c r="B109" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>231</v>
-      </c>
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="5"/>
       <c r="D109" s="5"/>
-      <c r="E109" s="7">
-        <v>177</v>
-      </c>
+      <c r="E109" s="7"/>
+      <c r="F109" s="5"/>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="16"/>
-      <c r="B110" s="16"/>
-      <c r="C110" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="D110" s="5"/>
-      <c r="E110" s="7">
-        <v>178</v>
-      </c>
+      <c r="A110" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E110" s="9"/>
       <c r="F110" s="5"/>
     </row>
     <row r="111" spans="1:6">
-      <c r="A111" s="6"/>
-      <c r="B111" s="6"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="7"/>
+      <c r="A111" t="s">
+        <v>248</v>
+      </c>
+      <c r="E111" s="9"/>
       <c r="F111" s="5"/>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="3" t="s">
-        <v>252</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C112" s="1"/>
       <c r="E112" s="9"/>
       <c r="F112" s="5"/>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" t="s">
-        <v>250</v>
-      </c>
-      <c r="E113" s="9"/>
+      <c r="A113" s="8"/>
+      <c r="B113" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>237</v>
+      </c>
       <c r="F113" s="5"/>
     </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C114" s="1"/>
-      <c r="E114" s="9"/>
+    <row r="114" spans="1:6" ht="30">
+      <c r="A114" s="5">
+        <v>1</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E114" s="7"/>
       <c r="F114" s="5"/>
     </row>
-    <row r="115" spans="1:6">
-      <c r="A115" s="8"/>
-      <c r="B115" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C115" s="8" t="s">
+    <row r="115" spans="1:6" ht="30">
+      <c r="A115" s="5">
+        <v>2</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E115" s="7"/>
+      <c r="F115" s="5"/>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="5">
         <v>3</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="F115" s="5"/>
-    </row>
-    <row r="116" spans="1:6" ht="30">
-      <c r="A116" s="5">
-        <v>1</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>171</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>267</v>
+        <v>172</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E116" s="7"/>
+        <v>232</v>
+      </c>
+      <c r="E116" s="7">
+        <v>152</v>
+      </c>
       <c r="F116" s="5"/>
     </row>
-    <row r="117" spans="1:6" ht="30">
+    <row r="117" spans="1:6">
       <c r="A117" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>218</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D117" s="5"/>
       <c r="E117" s="7"/>
       <c r="F117" s="5"/>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" ht="30">
       <c r="A118" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E118" s="7">
-        <v>152</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="D118" s="5"/>
+      <c r="E118" s="7"/>
       <c r="F118" s="5"/>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="5">
-        <v>4</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>175</v>
+      <c r="A119" s="15">
+        <v>6</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D119" s="5"/>
+      <c r="D119" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E119" s="7"/>
       <c r="F119" s="5"/>
     </row>
-    <row r="120" spans="1:6" ht="30">
-      <c r="A120" s="5">
-        <v>5</v>
-      </c>
-      <c r="B120" s="5" t="s">
+    <row r="120" spans="1:6">
+      <c r="A120" s="15"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C120" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D120" s="5"/>
+      <c r="D120" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E120" s="7"/>
       <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="16">
-        <v>6</v>
-      </c>
-      <c r="B121" s="16" t="s">
-        <v>15</v>
-      </c>
+      <c r="A121" s="15"/>
+      <c r="B121" s="15"/>
       <c r="C121" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E121" s="7"/>
       <c r="F121" s="5"/>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="16"/>
-      <c r="B122" s="16"/>
+      <c r="A122" s="15"/>
+      <c r="B122" s="15"/>
       <c r="C122" s="5" t="s">
         <v>179</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E122" s="7"/>
-      <c r="F122" s="5"/>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="16"/>
-      <c r="B123" s="16"/>
+      <c r="A123" s="15"/>
+      <c r="B123" s="15"/>
       <c r="C123" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E123" s="7"/>
-      <c r="F123" s="5"/>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="16"/>
-      <c r="B124" s="16"/>
+    </row>
+    <row r="124" spans="1:6" ht="30">
+      <c r="A124" s="15">
+        <v>7</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>215</v>
+      </c>
       <c r="C124" s="5" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E124" s="7"/>
+        <v>234</v>
+      </c>
+      <c r="E124" s="7">
+        <v>142</v>
+      </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="16"/>
-      <c r="B125" s="16"/>
+      <c r="A125" s="15"/>
+      <c r="B125" s="15"/>
       <c r="C125" s="5" t="s">
-        <v>182</v>
+        <v>235</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E125" s="7"/>
-    </row>
-    <row r="126" spans="1:6" ht="30">
-      <c r="A126" s="16">
-        <v>7</v>
-      </c>
-      <c r="B126" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="D126" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="E126" s="7">
-        <v>142</v>
-      </c>
+      <c r="E125" s="7">
+        <v>139</v>
+      </c>
+      <c r="F125" s="5"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="6"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="5"/>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="16"/>
-      <c r="B127" s="16"/>
-      <c r="C127" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="D127" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="E127" s="7">
-        <v>139</v>
+      <c r="A127" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="F127" s="5"/>
     </row>
     <row r="128" spans="1:6">
-      <c r="A128" s="6"/>
-      <c r="B128" s="6"/>
-      <c r="C128" s="5"/>
-      <c r="D128" s="5"/>
-      <c r="E128" s="7"/>
+      <c r="A128" t="s">
+        <v>248</v>
+      </c>
       <c r="F128" s="5"/>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" s="3" t="s">
-        <v>253</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C129" s="1"/>
       <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6">
-      <c r="A130" t="s">
-        <v>250</v>
+      <c r="A130" s="8"/>
+      <c r="B130" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>237</v>
       </c>
       <c r="F130" s="5"/>
     </row>
-    <row r="131" spans="1:6">
-      <c r="A131" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C131" s="1"/>
+    <row r="131" spans="1:6" ht="30">
+      <c r="A131" s="5">
+        <v>1</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E131" s="5"/>
       <c r="F131" s="5"/>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" s="8"/>
-      <c r="B132" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C132" s="8" t="s">
+      <c r="A132" s="5">
+        <v>2</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="15">
         <v>3</v>
       </c>
-      <c r="D132" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E132" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="F132" s="5"/>
-    </row>
-    <row r="133" spans="1:6" ht="30">
-      <c r="A133" s="5">
-        <v>1</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>183</v>
+      <c r="B133" s="15" t="s">
+        <v>182</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="D133" s="5" t="s">
-        <v>218</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="D133" s="5"/>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
     </row>
     <row r="134" spans="1:6">
-      <c r="A134" s="5">
-        <v>2</v>
-      </c>
-      <c r="B134" s="5" t="s">
-        <v>213</v>
-      </c>
+      <c r="A134" s="15"/>
+      <c r="B134" s="15"/>
       <c r="C134" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
     </row>
     <row r="135" spans="1:6">
-      <c r="A135" s="16">
-        <v>3</v>
-      </c>
-      <c r="B135" s="16" t="s">
-        <v>184</v>
-      </c>
+      <c r="A135" s="15"/>
+      <c r="B135" s="15"/>
       <c r="C135" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="D135" s="5"/>
+        <v>183</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
     </row>
     <row r="136" spans="1:6">
-      <c r="A136" s="16"/>
-      <c r="B136" s="16"/>
+      <c r="A136" s="15"/>
+      <c r="B136" s="15"/>
       <c r="C136" s="5" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
     </row>
     <row r="137" spans="1:6">
-      <c r="A137" s="16"/>
-      <c r="B137" s="16"/>
+      <c r="A137" s="15"/>
+      <c r="B137" s="15"/>
       <c r="C137" s="5" t="s">
         <v>185</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
     </row>
     <row r="138" spans="1:6">
-      <c r="A138" s="16"/>
-      <c r="B138" s="16"/>
+      <c r="A138" s="15"/>
+      <c r="B138" s="15"/>
       <c r="C138" s="5" t="s">
         <v>186</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" s="16"/>
-      <c r="B139" s="16"/>
+      <c r="A139" s="15"/>
+      <c r="B139" s="15"/>
       <c r="C139" s="5" t="s">
         <v>187</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="16"/>
-      <c r="B140" s="16"/>
+      <c r="A140" s="15"/>
+      <c r="B140" s="15"/>
       <c r="C140" s="5" t="s">
         <v>188</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
     </row>
     <row r="141" spans="1:6">
-      <c r="A141" s="16"/>
-      <c r="B141" s="16"/>
+      <c r="A141" s="15"/>
+      <c r="B141" s="15"/>
       <c r="C141" s="5" t="s">
         <v>189</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="16"/>
-      <c r="B142" s="16"/>
+      <c r="A142" s="15"/>
+      <c r="B142" s="15"/>
       <c r="C142" s="5" t="s">
         <v>190</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="16"/>
-      <c r="B143" s="16"/>
+      <c r="A143" s="15"/>
+      <c r="B143" s="15"/>
       <c r="C143" s="5" t="s">
         <v>191</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="16"/>
-      <c r="B144" s="16"/>
+      <c r="A144" s="15"/>
+      <c r="B144" s="15"/>
       <c r="C144" s="5" t="s">
         <v>192</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E144" s="5"/>
       <c r="F144" s="5"/>
     </row>
     <row r="145" spans="1:6">
-      <c r="A145" s="16"/>
-      <c r="B145" s="16"/>
+      <c r="A145" s="15"/>
+      <c r="B145" s="15"/>
       <c r="C145" s="5" t="s">
         <v>193</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E145" s="5"/>
       <c r="F145" s="5"/>
     </row>
     <row r="146" spans="1:6">
-      <c r="A146" s="16"/>
-      <c r="B146" s="16"/>
+      <c r="A146" s="15"/>
+      <c r="B146" s="15"/>
       <c r="C146" s="5" t="s">
         <v>194</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
     </row>
     <row r="147" spans="1:6">
-      <c r="A147" s="16"/>
-      <c r="B147" s="16"/>
+      <c r="A147" s="15"/>
+      <c r="B147" s="15"/>
       <c r="C147" s="5" t="s">
         <v>195</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E147" s="5"/>
       <c r="F147" s="5"/>
     </row>
     <row r="148" spans="1:6">
-      <c r="A148" s="16"/>
-      <c r="B148" s="16"/>
+      <c r="A148" s="15"/>
+      <c r="B148" s="15"/>
       <c r="C148" s="5" t="s">
         <v>196</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
     </row>
     <row r="149" spans="1:6">
-      <c r="A149" s="16"/>
-      <c r="B149" s="16"/>
+      <c r="A149" s="15"/>
+      <c r="B149" s="15"/>
       <c r="C149" s="5" t="s">
         <v>197</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
     </row>
     <row r="150" spans="1:6">
-      <c r="A150" s="16"/>
-      <c r="B150" s="16"/>
+      <c r="A150" s="15"/>
+      <c r="B150" s="15"/>
       <c r="C150" s="5" t="s">
         <v>198</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E150" s="5"/>
       <c r="F150" s="5"/>
     </row>
     <row r="151" spans="1:6">
-      <c r="A151" s="16"/>
-      <c r="B151" s="16"/>
+      <c r="A151" s="15"/>
+      <c r="B151" s="15"/>
       <c r="C151" s="5" t="s">
         <v>199</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E151" s="5"/>
       <c r="F151" s="5"/>
     </row>
     <row r="152" spans="1:6">
-      <c r="A152" s="16"/>
-      <c r="B152" s="16"/>
+      <c r="A152" s="15"/>
+      <c r="B152" s="15"/>
       <c r="C152" s="5" t="s">
         <v>200</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E152" s="5"/>
       <c r="F152" s="5"/>
     </row>
     <row r="153" spans="1:6">
-      <c r="A153" s="16"/>
-      <c r="B153" s="16"/>
+      <c r="A153" s="15"/>
+      <c r="B153" s="15"/>
       <c r="C153" s="5" t="s">
         <v>201</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
     </row>
     <row r="154" spans="1:6">
-      <c r="A154" s="16"/>
-      <c r="B154" s="16"/>
+      <c r="A154" s="15"/>
+      <c r="B154" s="15"/>
       <c r="C154" s="5" t="s">
         <v>202</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E154" s="5"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6">
-      <c r="A155" s="16"/>
-      <c r="B155" s="16"/>
+      <c r="A155" s="15"/>
+      <c r="B155" s="15"/>
       <c r="C155" s="5" t="s">
         <v>203</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6">
-      <c r="A156" s="16"/>
-      <c r="B156" s="16"/>
+      <c r="A156" s="15"/>
+      <c r="B156" s="15"/>
       <c r="C156" s="5" t="s">
         <v>204</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6">
-      <c r="A157" s="16"/>
-      <c r="B157" s="16"/>
+      <c r="A157" s="15"/>
+      <c r="B157" s="15"/>
       <c r="C157" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E157" s="5"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6">
-      <c r="A158" s="16"/>
-      <c r="B158" s="16"/>
+      <c r="A158" s="15">
+        <v>4</v>
+      </c>
+      <c r="B158" s="15" t="s">
+        <v>207</v>
+      </c>
       <c r="C158" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D158" s="5" t="s">
-        <v>218</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="D158" s="5"/>
       <c r="E158" s="5"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6">
-      <c r="A159" s="16"/>
-      <c r="B159" s="16"/>
+      <c r="A159" s="15"/>
+      <c r="B159" s="15"/>
       <c r="C159" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E159" s="5"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6">
-      <c r="A160" s="16">
-        <v>4</v>
-      </c>
-      <c r="B160" s="16" t="s">
+      <c r="A160" s="15"/>
+      <c r="B160" s="15"/>
+      <c r="C160" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C160" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="D160" s="5"/>
+      <c r="D160" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E160" s="5"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6">
-      <c r="A161" s="16"/>
-      <c r="B161" s="16"/>
+      <c r="A161" s="15"/>
+      <c r="B161" s="15"/>
       <c r="C161" s="5" t="s">
         <v>210</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E161" s="5"/>
       <c r="F161" s="5"/>
     </row>
-    <row r="162" spans="1:6">
-      <c r="A162" s="16"/>
-      <c r="B162" s="16"/>
+    <row r="162" spans="1:6" ht="45">
+      <c r="A162" s="5">
+        <v>5</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="C162" s="5" t="s">
-        <v>211</v>
+        <v>268</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E162" s="5"/>
       <c r="F162" s="5"/>
     </row>
     <row r="163" spans="1:6">
-      <c r="A163" s="16"/>
-      <c r="B163" s="16"/>
-      <c r="C163" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D163" s="5" t="s">
-        <v>218</v>
-      </c>
+      <c r="A163" s="5"/>
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
       <c r="E163" s="5"/>
       <c r="F163" s="5"/>
     </row>
-    <row r="164" spans="1:6" ht="45">
-      <c r="A164" s="5">
-        <v>5</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D164" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E164" s="5"/>
+    <row r="164" spans="1:6">
+      <c r="A164" s="3" t="s">
+        <v>279</v>
+      </c>
       <c r="F164" s="5"/>
     </row>
     <row r="165" spans="1:6">
-      <c r="A165" s="5"/>
-      <c r="B165" s="5"/>
-      <c r="C165" s="5"/>
-      <c r="D165" s="5"/>
-      <c r="E165" s="5"/>
+      <c r="A165" t="s">
+        <v>280</v>
+      </c>
       <c r="F165" s="5"/>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="3" t="s">
         <v>281</v>
       </c>
+      <c r="C166" s="1"/>
       <c r="F166" s="5"/>
     </row>
     <row r="167" spans="1:6">
-      <c r="A167" t="s">
-        <v>282</v>
+      <c r="A167" s="8"/>
+      <c r="B167" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C167" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D167" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>237</v>
       </c>
       <c r="F167" s="5"/>
     </row>
-    <row r="168" spans="1:6">
-      <c r="A168" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C168" s="1"/>
+    <row r="168" spans="1:6" ht="30">
+      <c r="A168" s="10">
+        <v>1</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C168" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D168" s="5"/>
+      <c r="E168" s="5"/>
       <c r="F168" s="5"/>
     </row>
-    <row r="169" spans="1:6">
-      <c r="A169" s="8"/>
-      <c r="B169" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C169" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D169" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E169" s="8" t="s">
-        <v>239</v>
-      </c>
+    <row r="169" spans="1:6" ht="30">
+      <c r="A169" s="10">
+        <v>2</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C169" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
       <c r="F169" s="5"/>
     </row>
     <row r="170" spans="1:6" ht="30">
       <c r="A170" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D170" s="5"/>
       <c r="E170" s="5"/>
       <c r="F170" s="5"/>
     </row>
-    <row r="171" spans="1:6" ht="30">
+    <row r="171" spans="1:6" ht="60">
       <c r="A171" s="10">
-        <v>2</v>
-      </c>
-      <c r="B171" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B171" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C171" s="12" t="s">
@@ -4508,416 +4545,410 @@
       </c>
       <c r="D171" s="5"/>
       <c r="E171" s="5"/>
-      <c r="F171" s="5"/>
-    </row>
-    <row r="172" spans="1:6" ht="30">
+    </row>
+    <row r="172" spans="1:6" ht="54" customHeight="1">
       <c r="A172" s="10">
-        <v>3</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>81</v>
+        <v>5</v>
+      </c>
+      <c r="B172" s="12" t="s">
+        <v>282</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D172" s="5"/>
-      <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
-    </row>
-    <row r="173" spans="1:6" ht="60">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173" s="10">
-        <v>4</v>
-      </c>
-      <c r="B173" s="12" t="s">
-        <v>70</v>
+        <v>6</v>
+      </c>
+      <c r="B173" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D173" s="5"/>
-      <c r="E173" s="5"/>
-    </row>
-    <row r="174" spans="1:6" ht="54" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
       <c r="A174" s="10">
-        <v>5</v>
-      </c>
-      <c r="B174" s="12" t="s">
-        <v>284</v>
+        <v>7</v>
+      </c>
+      <c r="B174" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="175" spans="1:6">
-      <c r="A175" s="10">
-        <v>6</v>
-      </c>
-      <c r="B175" s="11" t="s">
-        <v>75</v>
+      <c r="A175" s="17">
+        <v>8</v>
+      </c>
+      <c r="B175" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:6">
-      <c r="A176" s="10">
-        <v>7</v>
-      </c>
-      <c r="B176" s="11" t="s">
-        <v>77</v>
-      </c>
+      <c r="A176" s="17"/>
+      <c r="B176" s="16"/>
       <c r="C176" s="12" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
     </row>
     <row r="177" spans="1:5">
-      <c r="A177" s="18">
-        <v>8</v>
-      </c>
-      <c r="B177" s="17" t="s">
-        <v>15</v>
-      </c>
+      <c r="A177" s="17"/>
+      <c r="B177" s="16"/>
       <c r="C177" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="18"/>
-      <c r="B178" s="17"/>
+      <c r="A178" s="17"/>
+      <c r="B178" s="16"/>
       <c r="C178" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:5">
-      <c r="A179" s="18"/>
-      <c r="B179" s="17"/>
+      <c r="A179" s="17"/>
+      <c r="B179" s="16"/>
       <c r="C179" s="12" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
     </row>
     <row r="180" spans="1:5">
-      <c r="A180" s="18"/>
-      <c r="B180" s="17"/>
+      <c r="A180" s="17"/>
+      <c r="B180" s="16"/>
       <c r="C180" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="181" spans="1:5">
-      <c r="A181" s="18"/>
-      <c r="B181" s="17"/>
+      <c r="A181" s="17"/>
+      <c r="B181" s="16"/>
       <c r="C181" s="12" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
     </row>
     <row r="182" spans="1:5">
-      <c r="A182" s="18"/>
-      <c r="B182" s="17"/>
+      <c r="A182" s="17"/>
+      <c r="B182" s="16"/>
       <c r="C182" s="12" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="18"/>
-      <c r="B183" s="17"/>
+      <c r="A183" s="10">
+        <v>9</v>
+      </c>
+      <c r="B183" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="C183" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="184" spans="1:5">
-      <c r="A184" s="18"/>
-      <c r="B184" s="17"/>
+      <c r="A184" s="10">
+        <v>10</v>
+      </c>
+      <c r="B184" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="C184" s="12" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="185" spans="1:5">
-      <c r="A185" s="10">
-        <v>9</v>
-      </c>
-      <c r="B185" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C185" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="A185" s="10"/>
+      <c r="B185" s="11"/>
+      <c r="C185" s="12"/>
     </row>
     <row r="186" spans="1:5">
-      <c r="A186" s="10">
-        <v>10</v>
-      </c>
-      <c r="B186" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C186" s="12" t="s">
-        <v>27</v>
+      <c r="A186" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="187" spans="1:5">
-      <c r="A187" s="10"/>
-      <c r="B187" s="11"/>
-      <c r="C187" s="12"/>
+      <c r="A187" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="3" t="s">
-        <v>288</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="C188" s="1"/>
     </row>
     <row r="189" spans="1:5">
-      <c r="A189" t="s">
-        <v>282</v>
+      <c r="A189" s="8"/>
+      <c r="B189" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C189" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D189" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E189" s="8" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="190" spans="1:5">
-      <c r="A190" s="3" t="s">
+      <c r="A190" s="10">
+        <v>1</v>
+      </c>
+      <c r="B190" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C190" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D190" s="12"/>
+    </row>
+    <row r="191" spans="1:5" ht="30">
+      <c r="A191" s="10">
+        <v>2</v>
+      </c>
+      <c r="B191" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C191" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D191" s="12"/>
+    </row>
+    <row r="192" spans="1:5" ht="30">
+      <c r="A192" s="10">
+        <v>3</v>
+      </c>
+      <c r="B192" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C192" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D192" s="12"/>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="10">
+        <v>4</v>
+      </c>
+      <c r="B193" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C193" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D193" s="12"/>
+    </row>
+    <row r="194" spans="1:5" ht="30">
+      <c r="A194" s="10">
+        <v>5</v>
+      </c>
+      <c r="B194" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C194" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D194" s="12"/>
+    </row>
+    <row r="195" spans="1:5" ht="45">
+      <c r="A195" s="10">
+        <v>6</v>
+      </c>
+      <c r="B195" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="C190" s="1"/>
-    </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="8"/>
-      <c r="B191" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C191" s="8" t="s">
+      <c r="C195" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D195" s="12"/>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="10">
+        <v>7</v>
+      </c>
+      <c r="B196" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C196" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D196" s="12"/>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="10">
+        <v>8</v>
+      </c>
+      <c r="B197" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C197" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D197" s="12"/>
+    </row>
+    <row r="198" spans="1:5" ht="30">
+      <c r="A198" s="10">
+        <v>9</v>
+      </c>
+      <c r="B198" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C198" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="D198" s="12"/>
+    </row>
+    <row r="199" spans="1:5" ht="30">
+      <c r="A199" s="10">
+        <v>10</v>
+      </c>
+      <c r="B199" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C199" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D199" s="12"/>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="10">
+        <v>12</v>
+      </c>
+      <c r="B200" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C200" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D200" s="12"/>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="10">
+        <v>13</v>
+      </c>
+      <c r="B201" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C201" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D201" s="12"/>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="10">
+        <v>14</v>
+      </c>
+      <c r="B202" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C202" s="12"/>
+      <c r="D202" s="12"/>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="10"/>
+      <c r="B203" s="12"/>
+      <c r="C203" s="12"/>
+      <c r="D203" s="12"/>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C206" s="1"/>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="8"/>
+      <c r="B207" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C207" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D191" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E191" s="8" t="s">
+      <c r="D207" s="8" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="10">
+      <c r="E207" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208">
         <v>1</v>
       </c>
-      <c r="B192" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C192" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D192" s="12"/>
-    </row>
-    <row r="193" spans="1:4" ht="30">
-      <c r="A193" s="10">
+      <c r="B208" t="s">
+        <v>98</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209">
         <v>2</v>
       </c>
-      <c r="B193" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C193" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D193" s="12"/>
-    </row>
-    <row r="194" spans="1:4" ht="30">
-      <c r="A194" s="10">
-        <v>3</v>
-      </c>
-      <c r="B194" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C194" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D194" s="12"/>
-    </row>
-    <row r="195" spans="1:4">
-      <c r="A195" s="10">
-        <v>4</v>
-      </c>
-      <c r="B195" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C195" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D195" s="12"/>
-    </row>
-    <row r="196" spans="1:4" ht="30">
-      <c r="A196" s="10">
-        <v>5</v>
-      </c>
-      <c r="B196" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C196" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D196" s="12"/>
-    </row>
-    <row r="197" spans="1:4" ht="45">
-      <c r="A197" s="10">
-        <v>6</v>
-      </c>
-      <c r="B197" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="C197" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="D197" s="12"/>
-    </row>
-    <row r="198" spans="1:4">
-      <c r="A198" s="10">
-        <v>7</v>
-      </c>
-      <c r="B198" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C198" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D198" s="12"/>
-    </row>
-    <row r="199" spans="1:4">
-      <c r="A199" s="10">
-        <v>8</v>
-      </c>
-      <c r="B199" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C199" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D199" s="12"/>
-    </row>
-    <row r="200" spans="1:4" ht="30">
-      <c r="A200" s="10">
-        <v>9</v>
-      </c>
-      <c r="B200" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C200" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="D200" s="12"/>
-    </row>
-    <row r="201" spans="1:4" ht="30">
-      <c r="A201" s="10">
-        <v>10</v>
-      </c>
-      <c r="B201" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C201" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D201" s="12"/>
-    </row>
-    <row r="202" spans="1:4">
-      <c r="A202" s="10">
-        <v>12</v>
-      </c>
-      <c r="B202" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C202" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D202" s="12"/>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" s="10">
-        <v>13</v>
-      </c>
-      <c r="B203" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C203" s="12" t="s">
+      <c r="B209" t="s">
         <v>50</v>
       </c>
-      <c r="D203" s="12"/>
-    </row>
-    <row r="204" spans="1:4">
-      <c r="A204" s="10">
-        <v>14</v>
-      </c>
-      <c r="B204" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C204" s="12"/>
-      <c r="D204" s="12"/>
-    </row>
-    <row r="205" spans="1:4">
-      <c r="A205" s="10"/>
-      <c r="B205" s="12"/>
-      <c r="C205" s="12"/>
-      <c r="D205" s="12"/>
-    </row>
-    <row r="206" spans="1:4">
-      <c r="A206" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4">
-      <c r="A207" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4">
-      <c r="A208" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C208" s="1"/>
-    </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="8"/>
-      <c r="B209" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C209" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D209" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E209" s="8" t="s">
-        <v>239</v>
+      <c r="C209" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="210" spans="1:5">
       <c r="A210">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B210" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="211" spans="1:5">
       <c r="A211">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B211" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B212" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="213" spans="1:5">
       <c r="A213">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B213" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>106</v>
@@ -4925,10 +4956,10 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B214" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>110</v>
@@ -4936,127 +4967,129 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B215" t="s">
-        <v>109</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>108</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C215" s="2"/>
     </row>
     <row r="216" spans="1:5">
-      <c r="A216">
-        <v>7</v>
-      </c>
-      <c r="B216" t="s">
-        <v>111</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="C216" s="2"/>
     </row>
     <row r="217" spans="1:5">
-      <c r="A217">
-        <v>7</v>
-      </c>
-      <c r="B217" t="s">
-        <v>62</v>
-      </c>
-      <c r="C217" s="2"/>
+      <c r="A217" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="218" spans="1:5">
-      <c r="C218" s="2"/>
+      <c r="A218" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="3" t="s">
-        <v>289</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="C219" s="1"/>
     </row>
     <row r="220" spans="1:5">
-      <c r="A220" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5">
-      <c r="A221" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C221" s="1"/>
-    </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="8"/>
-      <c r="B222" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C222" s="8" t="s">
+      <c r="A220" s="8"/>
+      <c r="B220" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C220" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D222" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E222" s="8" t="s">
+      <c r="D220" s="8" t="s">
         <v>239</v>
       </c>
+      <c r="E220" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="30">
+      <c r="A221" s="14">
+        <v>1</v>
+      </c>
+      <c r="B221" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C221" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D221" s="12"/>
+      <c r="E221" s="13"/>
+    </row>
+    <row r="222" spans="1:5" ht="30">
+      <c r="A222" s="14">
+        <v>2</v>
+      </c>
+      <c r="B222" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C222" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D222" s="12"/>
+      <c r="E222" s="13"/>
     </row>
     <row r="223" spans="1:5" ht="30">
       <c r="A223" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B223" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D223" s="12"/>
       <c r="E223" s="13"/>
     </row>
     <row r="224" spans="1:5" ht="30">
       <c r="A224" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B224" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C224" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D224" s="12"/>
       <c r="E224" s="13"/>
     </row>
     <row r="225" spans="1:5" ht="30">
       <c r="A225" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D225" s="12"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="30">
+    <row r="226" spans="1:5">
       <c r="A226" s="14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B226" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C226" s="12" t="s">
-        <v>120</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C226" s="12"/>
       <c r="D226" s="12"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="30">
+    <row r="227" spans="1:5">
       <c r="A227" s="14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="C227" s="12" t="s">
         <v>122</v>
@@ -5066,59 +5099,35 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C228" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C228" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="D228" s="12"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5">
-      <c r="A229" s="14">
-        <v>7</v>
-      </c>
-      <c r="B229" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C229" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D229" s="12"/>
-      <c r="E229" s="13"/>
-    </row>
-    <row r="230" spans="1:5">
-      <c r="A230" s="14">
-        <v>8</v>
-      </c>
-      <c r="B230" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C230" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D230" s="12"/>
-      <c r="E230" s="13"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B177:B184"/>
-    <mergeCell ref="A177:A184"/>
-    <mergeCell ref="A160:A163"/>
-    <mergeCell ref="B160:B163"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="B121:B125"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B135:B159"/>
-    <mergeCell ref="A135:A159"/>
-    <mergeCell ref="B15:B22"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="B104:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="B133:B157"/>
+    <mergeCell ref="A133:A157"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B175:B182"/>
+    <mergeCell ref="A175:A182"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="B158:B161"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="B119:B123"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>